<commit_message>
added new country description
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\5_Research\WP1\Collected Data\3_working data\shiny_countries-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CA876A-10D8-48E8-B8C5-1031E195DD22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97B9938-D431-403D-9693-AFBAC1DE9445}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="5604" xr2:uid="{846E64D6-5A33-41DE-910F-6786C3520ECE}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>actor</t>
   </si>
@@ -117,13 +117,7 @@
     <t>http://www.marenet.de/MareNet/europe.html</t>
   </si>
   <si>
-    <t xml:space="preserve">In the EU there are about 230 research institutes out of which 55 are located in the UK, 46 in Germany and 29 in France [1]. There are currently 99 research vessels  in Europe which are run 62 different research vessel operators in 23 countries [2]. Nevertheless, the distribution of vessels in Europe is not uniform. Three countries each operate 11 vessels (France, Germany and Norway), three countries operate between 7 and 9 vessels (UK, Spain and Portugal), and the remaining 17 countries operate five vessels or fewer [2]. </t>
-  </si>
-  <si>
     <t>manual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the BBNJ negotiations, Brazil is part of the Core Latin American Countries Group and represents the groups positions in matters relating to MGRs. </t>
   </si>
   <si>
     <t>text_science</t>
@@ -146,6 +140,39 @@
 [4] http://www.uff.br/?q=noticias/06-11-2018/navio-escola-da-uff-ampliara-desenvolvimento-tecnologico-nas-ciencias-do-mar
 [5] https://tapioca.ird.fr/embarcacao-ciencias-mar-iv-chega-neste-semestre-ao-porto-recife/
 [6] https://www.marinha.mil.br/secirm/psrm/ppgmar</t>
+  </si>
+  <si>
+    <t>Within the UN framework, Brazil forms part of the Latin American and Carribean group of states but during the second Intergovernmental Conference (IGC 2) it negotiated through the group of Likeminded Latin American Countries. Because during IGC 1 Brazil and other Latin American countries still stated their individual preferences, it is concluded that the Latin American and likeminded Group formed particularly for the BBNJ process between IGC 1 and 2. The group of Like-Minded Latin American Countries consisted of Argentina, Brazil, Colombia, Costa Rica, Ecuador, El Salvador, Guatemala, Honduras, Mexico, Panama, Paraguay, Peru, Dominican Republic and Uruguay.
+Brazil spoke for the Like-Minded Latin American Countries group on Marine Genetic Resources (MGRs); Argentina on Area Based Management Tools (ABMTs) including Marine Protected Areas (MPAs); Uruguay on Environmental Impact Assessments (EIAs); Honduras on Capacity Building and Technology Transfer (CBTT) and Colombia on Cross-Cutting Issues. 
+MGRs
+In IGC 2 Brazil acted through the Likeminded Latin American Countries. The Brazilian Delegate Barbara Boechat was the spokesperson on behalf of the Group on the topic of MGRs. On MGRs, Brazil made clear that the Latin American and Liked-Minded Countries group preferred an option including the sharing of both monetary and non-monetary benefits, noting that only “voluntary benefits” is not workable. Brazil also argued that the principle of “common heritage of mankind” should be included in the section concerning the governing principles of benefit sharing not only for MGRs but for the whole treaty. Concerning the objectives and technicalities of benefit sharing modalities, Brazil stated on behalf of Like-Minded Latin American Countries and supported by the Republic Of Korea, that an overarching section on objectives including principles and approaches including a provision on a strong Clearing-House Mechanism (CHM) is preferable. On behalf of the Like-Minded Latin American Countries, Brazil supported the development of a non-exhaustive list of benefits within the treaty, as opposed to a list being developed at a later stage as well as the inclusion of monitoring measures by the CHM.
+ABMTs:
+On the identification of areas, Argentina on behalf of the Likeminded Latin American Countries alongside the G-77/China, Caricom, Sri Lanka, The African Group, Singapore and the High Seas Alliances supported a non-exhaustive list of standards and criteria for the identification of areas. On the designation of ABMTs including MPAs, the Likeminded Latin American Countries Group favoured that a decision making body can decide on the designation of all ABMTs. Furthermore, the Like-Minded Latin American Countries recognizes that consultation with concerned states, including adjacent coastal states is important. Uruguay further made a statement in relation to the inclusion of the EBSAs for the designation of ABMTs. 
+EIAs: 
+Uruguay on behalf of the Likeminded Latin American Countries and supported by G-77/China, the African Group, EU, P-SIDS, CARICOM and Canada argued against postponing the development of the EIA process and in favour of outlining the steps for conducting an EIA in the treaty. Uruguay supported that the content of an EIA should be described as detailed as possible including the determination of whether an EIA is needed. On the activities that need an EIA, The Like-Minded Latin American Countries, supported by the US, Norway, Australia, New Zealand and India, preferred that states parties assess whether they activities cause substantial pollution. On cumulative impacts, the Like-Minded Latin American Countries alongside the EU, Japan and Norway favoured also considering these impacts. Concerning the monitoring and review process, the Likeminded Latin American Countries group argued that these provisions should be moved to the general section. 
+CBTT:
+On CBTT, Honduras on behalf of the Like-Minded Latin American Countries supported - alongside the G-77/CHINA, CARICOM, AOSIS, NEW ZEALAND and INDIA - the inclusion of a list of CBTT activities and an outline of the modalities in the body of the treaty. Concerning the possible development of a clearinghouse mechanism, the Like-Minded Latin American Countries supported setting out the functions of a clearinghouse mechanism, however noting that this issue is cross-cutting and should be included in a general section. On the discussion of funding types, the group of Like-Minded Latin American Countries alongside the African Group, the G-77/China, the EU, CARICOM and the P-SIDS agreed that funding should be both voluntary and mandatory (however the EU noting that mandatory funding should be restricted to institutional and clearinghouse mechanism costs).
+Cross-Cutting Issues:
+On Cross-Cutting Issues, Colombia on behalf of the Like-Minded Latin American Countries stated that the group supports the establishment of a Conference of Parties as a decision-making body while asking to clarify the functions and the composition of the body. Furthermore, the Group supports the establishment of a secretariat and shows flexibility on where such a body would reside. Interestingly, the Like-Minded Latin American Countries alongside the African Group suggested removing references to high seas freedoms under the “General Principles and Approaches” section.</t>
+  </si>
+  <si>
+    <t>The BBNJ Working Group started meeting in 2006 and the EU has been a strong promotor of this political process since its beginning calling for the adoption of an UNCLOS 1A (Druel &amp; Gjerde, 2014; European Commission, 2019). Nevertheless, this early idea did not include MGRs and failed to reach a global consensus to sustain negotiations and therefore it took up an increased political interests only after 2009 (own interview, 2019). 
+The EU represents a broad field of interested states in the negotiations that consistently negotiate under a common mandate. 
+MGRs
+The EU’s delegate diverted from the strict naming-naming-of-options method of negotiation and made a more logical argument based statement, emphasizing that the EU favours a “holistic approach” for MGRs. The statements focussed on operationalizing the provisions of the treaty on the sharing of information, scientific data, and knowledge and the building of research capacities. The EU delegate reiterated that the EU does not support addressing intellectual property rights under the new treaty (supported by the US, Switzerland, Norway, Holy See, Japan, The Republic of Korea, The Russian Federation and Australia). The EU also stated that fish or other biological commodities should not be addressed. It was noted that activities related to MGRs are in essence marine scientific research, which should not be hampered in any way. It was argued that the clearing house is a cross-cutting issue in itself and Anca Leroy rejecting a possible connection to Nagoya in the treaty text.
+ABMTs:
+The EU alongside Micronesia, Cameroon, New Zealand, and the High Seas Alliance favoured reference to traditional knowledge as an additional source of information but remained critical to the inclusion of economic and social factors in the identification of areas. The EU strongly supported the application of the precautionary principle, the ecosystem approach and a reference to best available science whereas the US, Singapore, Australia, Canada and Japan favoured the precautionary approach. It was explained that a lack of scientific knowledge should not justify taking no protecting measures. Furthermore, the EU supported the establishment of a connected network of MPAs. Proposals of ABMTs should be reviewed by a scientific/technical body and designated by a COP which would also possess the authority of the designated area.
+EIAs: 
+The EU as well as the Likeminded Latin American Countries, G-77/China, the African Group, P-SIDS, CARICOM and Canada supported the outlining the steps, albeit in a little detailed manner, for conducting an EIA in the treaty as opposed to establish the process later on. The EU supported requiring a description of planned activities as well as a description of reasonable alternatives in an EIA. Under descriptions of impacts, the EU, alongside P-SIDS, the US, India, Norway, Indonesia, Canada and the African Group supported describing effects, including cumulative and transboundary impacts. The EU furthermore made a reference to the CBD for detailed guidelines on EIAs and noted that EBSAs can be helpful to determine the location and characterization of the ecosystem. Finally, the EU, with many others, argued that compliance should be taken up under cross-cutting issues and favoured an activity-based approach to defining the threshold for an EIA.
+CBTT:
+On CBTT, the EU noted that the list of types and modalities is too long. Nevertheless, the EU agreed with the African Group, the G-77/CHINA, CARICOM, the Like-Minded Latin American Countries, and P-SIDS that funding should be both voluntary and mandatory, with the EU underlining that mandatory funding be restricted to institutional and clearinghouse mechanism costs. On sources, the EU called for including national funding sources, and P-SIDS welcomed the inclusion of innovative funding sources. The EU proposed that a CHM can be established and supported the definition of functions and goals of a clearinghouse mechanism.
+Cross-Cutting Issues:
+Under Cross-Cutting Issues, a decision-making body or forum was discussed. The EU alongside the G-77/China, AOSIS, the African Group, Canada, Iceland and others supported establishing a COP under the implementing agreement and the EU noted that a provision on the first meeting of the COP should be explicitly included in the agreement. Concerning formulating the form and functions of the body, it was noted that it should be adequate to achieve the objectives, suggesting distinguishing between institutional and substantial functions. The EU supported the establishment of a scientific/technical body, preferring a scientific body and calling for flexibility to allow additional tasks to be mandated by the COP. The EU suggested the development of a pool of independent scientific experts, but also using expertise from existing arrangements. The EU argued that the functioning of a CHM can be discussed by the following COP. Where the G-77/China, the African Group, P-SIDS an others called for the inclusion of common heritage of humankind as a general principle, the EU but remained open to the common heritage of mankind principle, clarifying that principles that need to be stated in general provisions and those which should be operationalized in special sections are separated. Concerning definitions, the EU referred to UNCLOS and CBD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Managing and preventing the loss of biodiversity became a political topic in the EU in the 1990s. The European Environment Agency (EEA) observed extensive biodiversity loss across the European Community in a report putting pressure on governments to commonly act against these developments (EEA, Report for the Review of the Fifth Environmental Action Programme, 1995). On a global level, the Commission listed the biodiversity loss as one of the seven serious environmental problems facing the Union (CEC, Europe’s Environment: What Directions for the Future? The Global Assessment of the European Community Programme of Policy and Action in Relation to the Environment and Sustainable Development: ‘Towards Sustainability’,1999). Accordingly, the European Community was not only a major force in the negotiation of the CBD but also signed it already in 1992.
+In 2010, the EU identified halting the global loss of biodiversity by 2020 as one of its key priorities. A review in 2015 found that although the EU is the largest financial donor and has increased resources for global biodiversity, current progress is insufficient in reducing the impacts of EU consumption patterns on global biodiversity (EU, Biodiversity Strategy 2020 Midterm Review, 2015). The EU has been a supporter of multilateral approaches, openly addressing developing countries concerns about the fair and equitable sharing of benefits and as such it played an active role in the negotiation of the Nagoya Protocol. 
+In the EU there are about 230 research institutes out of which 55 are located in the UK, 46 in Germany and 29 in France [1]. There are currently 99 research vessels  in Europe which are run 62 different research vessel operators in 23 countries [2]. Nevertheless, the distribution of vessels in Europe is not uniform. Three countries each operate 11 vessels (France, Germany and Norway), three countries operate between 7 and 9 vessels (UK, Spain and Portugal), and the remaining 17 countries operate five vessels or fewer [2]. </t>
   </si>
 </sst>
 </file>
@@ -644,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6B521D-785F-49AC-BCBD-36F7078EDED3}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,13 +686,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -682,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -698,15 +725,18 @@
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>11</v>
@@ -719,18 +749,18 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" ht="403.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="18" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="20"/>

</xml_diff>

<commit_message>
test <br>s in research xls
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -1,75 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\5_Research\WP1\Collected Data\3_working data\shiny_countries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64C73E9-2C65-4F99-A7C3-5825FC80C48C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="5604" xr2:uid="{846E64D6-5A33-41DE-910F-6786C3520ECE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="5610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Argyll" localSheetId="0">Sheet1!$G$20</definedName>
-    <definedName name="Bangor" localSheetId="0">Sheet1!$G$24</definedName>
-    <definedName name="Belgium" localSheetId="0">Sheet1!$G$15</definedName>
-    <definedName name="Bidston" localSheetId="0">Sheet1!$G$29</definedName>
-    <definedName name="Bracknell" localSheetId="0">Sheet1!$G$35</definedName>
-    <definedName name="Brighton" localSheetId="0">Sheet1!$G$40</definedName>
-    <definedName name="Cambrigde" localSheetId="0">Sheet1!$G$43</definedName>
-    <definedName name="Cardiff" localSheetId="0">Sheet1!$G$47</definedName>
-    <definedName name="Croatia" localSheetId="0">Sheet1!$G$44</definedName>
-    <definedName name="Denmark" localSheetId="0">Sheet1!$G$67</definedName>
-    <definedName name="Edinburgh" localSheetId="0">Sheet1!$G$52</definedName>
-    <definedName name="Estonia" localSheetId="0">Sheet1!$G$99</definedName>
-    <definedName name="Faeroe" localSheetId="0">Sheet1!$G$110</definedName>
-    <definedName name="Finland" localSheetId="0">Sheet1!$G$117</definedName>
-    <definedName name="France" localSheetId="0">Sheet1!$G$126</definedName>
-    <definedName name="Germany" localSheetId="0">Sheet1!$G$133</definedName>
-    <definedName name="Glasgow" localSheetId="0">Sheet1!$G$56</definedName>
-    <definedName name="Godalming" localSheetId="0">Sheet1!$G$62</definedName>
-    <definedName name="Greece" localSheetId="0">Sheet1!$G$140</definedName>
-    <definedName name="Hull" localSheetId="0">Sheet1!$G$65</definedName>
-    <definedName name="Iceland" localSheetId="0">Sheet1!$G$160</definedName>
-    <definedName name="Ireland" localSheetId="0">Sheet1!$G$171</definedName>
-    <definedName name="Israel" localSheetId="0">Sheet1!$G$193</definedName>
-    <definedName name="Italy" localSheetId="0">Sheet1!$G$207</definedName>
-    <definedName name="Liverpool" localSheetId="0">Sheet1!$G$69</definedName>
-    <definedName name="London" localSheetId="0">Sheet1!$G$79</definedName>
-    <definedName name="Londonderry" localSheetId="0">Sheet1!$G$85</definedName>
-    <definedName name="Lowestoft" localSheetId="0">Sheet1!$G$89</definedName>
-    <definedName name="Malta" localSheetId="0">Sheet1!$G$244</definedName>
-    <definedName name="Millport" localSheetId="0">Sheet1!$G$96</definedName>
-    <definedName name="Netherlands" localSheetId="0">Sheet1!$G$255</definedName>
-    <definedName name="Newcastle" localSheetId="0">Sheet1!$G$92</definedName>
-    <definedName name="Norway" localSheetId="0">Sheet1!$G$292</definedName>
-    <definedName name="Norwich" localSheetId="0">Sheet1!$G$99</definedName>
-    <definedName name="Other" localSheetId="0">Sheet1!$G$151</definedName>
-    <definedName name="Oxford" localSheetId="0">Sheet1!$G$103</definedName>
-    <definedName name="Plymouth" localSheetId="0">Sheet1!$G$109</definedName>
-    <definedName name="Poland" localSheetId="0">Sheet1!$G$330</definedName>
-    <definedName name="PortArthur" localSheetId="0">Sheet1!$G$117</definedName>
-    <definedName name="Portugal" localSheetId="0">Sheet1!$G$356</definedName>
-    <definedName name="Reading" localSheetId="0">Sheet1!$G$120</definedName>
-    <definedName name="Russia" localSheetId="0">Sheet1!$G$386</definedName>
-    <definedName name="Scarborough" localSheetId="0">Sheet1!$G$124</definedName>
-    <definedName name="Southampton" localSheetId="0">Sheet1!$G$128</definedName>
-    <definedName name="Spain" localSheetId="0">Sheet1!$G$404</definedName>
-    <definedName name="StAndrews" localSheetId="0">Sheet1!$G$137</definedName>
-    <definedName name="Stirling" localSheetId="0">Sheet1!$G$141</definedName>
-    <definedName name="Sweden" localSheetId="0">Sheet1!$G$462</definedName>
-    <definedName name="Swindon" localSheetId="0">Sheet1!$G$148</definedName>
-    <definedName name="top" localSheetId="0">Sheet1!$G$7</definedName>
-    <definedName name="Turkey" localSheetId="0">Sheet1!$G$497</definedName>
-    <definedName name="Ukraine" localSheetId="0">Sheet1!$G$506</definedName>
+    <definedName name="Argyll" localSheetId="0">Sheet1!$G$21</definedName>
+    <definedName name="Bangor" localSheetId="0">Sheet1!$G$25</definedName>
+    <definedName name="Belgium" localSheetId="0">Sheet1!$G$16</definedName>
+    <definedName name="Bidston" localSheetId="0">Sheet1!$G$30</definedName>
+    <definedName name="Bracknell" localSheetId="0">Sheet1!$G$36</definedName>
+    <definedName name="Brighton" localSheetId="0">Sheet1!$G$41</definedName>
+    <definedName name="Cambrigde" localSheetId="0">Sheet1!$G$44</definedName>
+    <definedName name="Cardiff" localSheetId="0">Sheet1!$G$48</definedName>
+    <definedName name="Croatia" localSheetId="0">Sheet1!$G$45</definedName>
+    <definedName name="Denmark" localSheetId="0">Sheet1!$G$68</definedName>
+    <definedName name="Edinburgh" localSheetId="0">Sheet1!$G$53</definedName>
+    <definedName name="Estonia" localSheetId="0">Sheet1!$G$100</definedName>
+    <definedName name="Faeroe" localSheetId="0">Sheet1!$G$111</definedName>
+    <definedName name="Finland" localSheetId="0">Sheet1!$G$118</definedName>
+    <definedName name="France" localSheetId="0">Sheet1!$G$127</definedName>
+    <definedName name="Germany" localSheetId="0">Sheet1!$G$134</definedName>
+    <definedName name="Glasgow" localSheetId="0">Sheet1!$G$57</definedName>
+    <definedName name="Godalming" localSheetId="0">Sheet1!$G$63</definedName>
+    <definedName name="Greece" localSheetId="0">Sheet1!$G$141</definedName>
+    <definedName name="Hull" localSheetId="0">Sheet1!$G$66</definedName>
+    <definedName name="Iceland" localSheetId="0">Sheet1!$G$161</definedName>
+    <definedName name="Ireland" localSheetId="0">Sheet1!$G$172</definedName>
+    <definedName name="Israel" localSheetId="0">Sheet1!$G$194</definedName>
+    <definedName name="Italy" localSheetId="0">Sheet1!$G$208</definedName>
+    <definedName name="Liverpool" localSheetId="0">Sheet1!$G$70</definedName>
+    <definedName name="London" localSheetId="0">Sheet1!$G$80</definedName>
+    <definedName name="Londonderry" localSheetId="0">Sheet1!$G$86</definedName>
+    <definedName name="Lowestoft" localSheetId="0">Sheet1!$G$90</definedName>
+    <definedName name="Malta" localSheetId="0">Sheet1!$G$245</definedName>
+    <definedName name="Millport" localSheetId="0">Sheet1!$G$97</definedName>
+    <definedName name="Netherlands" localSheetId="0">Sheet1!$G$256</definedName>
+    <definedName name="Newcastle" localSheetId="0">Sheet1!$G$93</definedName>
+    <definedName name="Norway" localSheetId="0">Sheet1!$G$293</definedName>
+    <definedName name="Norwich" localSheetId="0">Sheet1!$G$100</definedName>
+    <definedName name="Other" localSheetId="0">Sheet1!$G$152</definedName>
+    <definedName name="Oxford" localSheetId="0">Sheet1!$G$104</definedName>
+    <definedName name="Plymouth" localSheetId="0">Sheet1!$G$110</definedName>
+    <definedName name="Poland" localSheetId="0">Sheet1!$G$331</definedName>
+    <definedName name="PortArthur" localSheetId="0">Sheet1!$G$118</definedName>
+    <definedName name="Portugal" localSheetId="0">Sheet1!$G$357</definedName>
+    <definedName name="Reading" localSheetId="0">Sheet1!$G$121</definedName>
+    <definedName name="Russia" localSheetId="0">Sheet1!$G$387</definedName>
+    <definedName name="Scarborough" localSheetId="0">Sheet1!$G$125</definedName>
+    <definedName name="Southampton" localSheetId="0">Sheet1!$G$129</definedName>
+    <definedName name="Spain" localSheetId="0">Sheet1!$G$405</definedName>
+    <definedName name="StAndrews" localSheetId="0">Sheet1!$G$138</definedName>
+    <definedName name="Stirling" localSheetId="0">Sheet1!$G$142</definedName>
+    <definedName name="Sweden" localSheetId="0">Sheet1!$G$463</definedName>
+    <definedName name="Swindon" localSheetId="0">Sheet1!$G$149</definedName>
+    <definedName name="top" localSheetId="0">Sheet1!$G$8</definedName>
+    <definedName name="Turkey" localSheetId="0">Sheet1!$G$498</definedName>
+    <definedName name="Ukraine" localSheetId="0">Sheet1!$G$507</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="190">
   <si>
     <t>actor</t>
   </si>
@@ -143,13 +142,6 @@
 On CBTT, the EU noted that the list of types and modalities is too long. Nevertheless, the EU agreed with the African Group, the G-77/CHINA, CARICOM, the Like-Minded Latin American Countries, and P-SIDS that funding should be both voluntary and mandatory, with the EU underlining that mandatory funding be restricted to institutional and clearinghouse mechanism costs. On sources, the EU called for including national funding sources, and P-SIDS welcomed the inclusion of innovative funding sources. The EU proposed that a CHM can be established and supported the definition of functions and goals of a clearinghouse mechanism.
 Cross-Cutting Issues:
 Under Cross-Cutting Issues, a decision-making body or forum was discussed. The EU alongside the G-77/China, AOSIS, the African Group, Canada, Iceland and others supported establishing a COP under the implementing agreement and the EU noted that a provision on the first meeting of the COP should be explicitly included in the agreement. Concerning formulating the form and functions of the body, it was noted that it should be adequate to achieve the objectives, suggesting distinguishing between institutional and substantial functions. The EU supported the establishment of a scientific/technical body, preferring a scientific body and calling for flexibility to allow additional tasks to be mandated by the COP. The EU suggested the development of a pool of independent scientific experts, but also using expertise from existing arrangements. The EU argued that the functioning of a CHM can be discussed by the following COP. Where the G-77/China, the African Group, P-SIDS an others called for the inclusion of common heritage of humankind as a general principle, the EU but remained open to the common heritage of mankind principle, clarifying that principles that need to be stated in general provisions and those which should be operationalized in special sections are separated. Concerning definitions, the EU referred to UNCLOS and CBD.</t>
-  </si>
-  <si>
-    <t>Managing and preventing the loss of biodiversity became a political topic in the EU in the 1990s. The European Environment Agency (EEA) observed extensive biodiversity loss across the European Community in a report putting pressure on governments to commonly act against these developments (EEA, Report for the Review of the Fifth Environmental Action Programme, 1995). On a global level, the Commission listed the biodiversity loss as one of the seven serious environmental problems facing the Union (CEC, Europe’s Environment: What Directions for the Future? The Global Assessment of the European Community Programme of Policy and Action in Relation to the Environment and Sustainable Development: ‘Towards Sustainability’,1999). Accordingly, the European Community was not only a major force in the negotiation of the CBD but also signed it already in 1992.
-In 2010, the EU identified halting the global loss of biodiversity by 2020 as one of its key priorities. A review in 2015 found that although the EU is the largest financial donor and has increased resources for global biodiversity, current progress is insufficient in reducing the impacts of EU consumption patterns on global biodiversity (EU, Biodiversity Strategy 2020 Midterm Review, 2015). The EU has been a supporter of multilateral approaches, openly addressing developing countries concerns about the fair and equitable sharing of benefits and as such it played an active role in the negotiation of the Nagoya Protocol. 
-In the EU there are about 230 research institutes out of which 55 are located in the UK, 46 in Germany and 29 in France [1]. There are currently 99 research vessels in Europe which are run 62 different research vessel operators in 23 countries [2]. Nevertheless, the distribution of vessels in Europe is not uniform. Three countries each operate 11 vessels (France, Germany and Norway), three countries operate between 7 and 9 vessels (UK, Spain and Portugal), and the remaining 17 countries operate five vessels or fewer [2]. 
-[1] http://www.marenet.de/MareNet/europe.html 
-[2] https://www.marineboard.eu/sites/marineboard.eu/files/public/publication/EMB_PB7_Research_Vessels_Web_v4_0.pdf</t>
   </si>
   <si>
     <t>Brazil is a country with strong interests in ocean issues. Its Exclusive Economic Zone encompasses 4.5 million km2 - called the Blue Amazon (Amazonia Azul) - which equals over 50% of the country’s land surface. 
@@ -863,11 +855,30 @@
   <si>
     <t>The USA has an extensive network of ocean research facilities and labroratories. The National Association of Marine Labroratories counts with 104 member marine labroratories [1]. The various institutions in the USA are reported to posses marine research vessels, out of which NOAA posseses 19 and the US navy 10 vessels.</t>
   </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Managing and preventing the loss of biodiversity became a political topic in the EU in the 1990s. The European Environment Agency (EEA) observed extensive biodiversity loss across the European Community in a report putting pressure on governments to commonly act against these developments (EEA, Report for the Review of the Fifth Environmental Action Programme, 1995). On a global level, the Commission listed the biodiversity loss as one of the seven serious environmental problems facing the Union (CEC, Europe’s Environment: What Directions for the Future? The Global Assessment of the European Community Programme of Policy and Action in Relation to the Environment and Sustainable Development: ‘Towards Sustainability’,1999). Accordingly, the European Community was not only a major force in the negotiation of the CBD but also signed it already in 1992. &lt;br&gt;
+In 2010, the EU identified halting the global loss of biodiversity by 2020 as one of its key priorities. A review in 2015 found that although the EU is the largest financial donor and has increased resources for global biodiversity, current progress is insufficient in reducing the impacts of EU consumption patterns on global biodiversity (EU, Biodiversity Strategy 2020 Midterm Review, 2015). The EU has been a supporter of multilateral approaches, openly addressing developing countries concerns about the fair and equitable sharing of benefits and as such it played an active role in the negotiation of the Nagoya Protocol. &lt;br&gt;
+In the EU there are about 230 research institutes out of which 55 are located in the UK, 46 in Germany and 29 in France [1]. There are currently 99 research vessels in Europe which are run 62 different research vessel operators in 23 countries [2]. Nevertheless, the distribution of vessels in Europe is not uniform. Three countries each operate 11 vessels (France, Germany and Norway), three countries operate between 7 and 9 vessels (UK, Spain and Portugal), and the remaining 17 countries operate five vessels or fewer [2]. &lt;b&gt;
+[1] http://www.marenet.de/MareNet/europe.html 
+[2] https://www.marineboard.eu/sites/marineboard.eu/files/public/publication/EMB_PB7_Research_Vessels_Web_v4_0.pdf</t>
+  </si>
+  <si>
+    <t>Over one hundred governments are currently negotiating a new legally binding instrument for the conservation and sustainable use of marine biological diversity in areas beyond national jurisdiction (BBNJ). The new agreement is to address four broad themes: marine genetic resources (MGRs); area-based management tools (ABMTs), including marine protected areas (MPAs); environmental impact assessments (EIAs); and capacity building and the transfer of marine technology (CB&amp;TT).  &lt;a href="https://www.frontiersin.org/articles/10.3389/fmars.2020.614282/full"&gt;&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>International scientific collaboration is essential to support global and regional efforts to protect marine biodiversity in areas within and beyond national jurisdiction [24], [28], [11]. Several scientific programs and initiatives, such as the International Census of Marine Life Programme [13], [37] or the recently launched UN Decade of Ocean Science [59] take the need to enhance scientific cooperation across regions into account to close data gaps, align research programs, and support conservation efforts [3], [44]. &lt;br&gt;
+Marine biodiversity research spans different spatial and temporal scales to assess global biodiversity loss patterns and is considered one of the most complex scientific fields to have emerged in recent decades [10]. As a big science, it ties together research teams, scientific infrastructures, laboratories, and equipment from different countries and regions of the world [58]. While international scientific collaboration seems to be inherent to the marine biodiversity field, it is also highly encouraged by the United Nations Convention on the Law of the Sea (UNCLOS). &lt;br&gt;
+Under Article 242 of UNCLOS, “States and competent international organizations shall promote international cooperation in marine scientific research for peaceful purposes." Acknowledging “rapid advances being made in the field of marine science and technology," Annex 6 of UNCLOS “urges the industrialized countries to assist the developing countries in the preparation and implementation of their marine science, [and] technology" (UNCLOS 1992, Annex 6). While scientists and governments seem to agree that scientific cooperation is needed to reduce global imbalances in marine science, most notably by fostering capacity building and marine technology transfer (CBMTT), progress in defining and assessing “the special interests and needs of developing countries" (UNCLOS Preamble) has been slow [25]. &lt;br&gt;
+Research has shown that international scientific cooperation in marine scientific research benefits from the combination of regional and intra-regional scientific cooperation [19], [5] and efforts to foster CBMTT within the scientific communities themselves [25], [35]. CBMTT is especially relevant regarding marine biodiversity in areas beyond national jurisdiction (BBNJ), where enhanced international scientific cooperation may account for the lack of legal frameworks regulating marine biodiversity in the High Seas [24], [63]. In ongoing intergovernmental negotiations to establish a new legally binding instrument for the protection and sustainable use of BBNJ, states view capacity building as a measure to be “carried out through enhanced cooperation at all levels and in all forms [.]" [55]. However, the actual arrangement of scientific cooperation as a means of CBMTT remains a contentious issue, especially among states that have the means to conduct marine scientific research and those who have not, most notably governments form the global South and the group of the least developed countries [15], [56], [27].</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1057,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1163,17 +1174,20 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1484,22 +1498,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6B521D-785F-49AC-BCBD-36F7078EDED3}">
-  <dimension ref="A1:J155"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="121.6640625" customWidth="1"/>
-    <col min="3" max="3" width="128.77734375" customWidth="1"/>
-    <col min="4" max="4" width="136.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="121.7109375" customWidth="1"/>
+    <col min="3" max="3" width="128.7109375" customWidth="1"/>
+    <col min="4" max="4" width="136.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1519,186 +1533,184 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="B4" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="15" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="409.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>8</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="1"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" s="17" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:10" ht="409.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" s="17" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="C6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
-        <v>20</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="1"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="13"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="10"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="2"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
-        <v>25</v>
+    <row r="12" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
-        <v>26</v>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -1709,9 +1721,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -1722,16 +1734,12 @@
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>31</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="F16" s="9"/>
       <c r="G16" s="1"/>
@@ -1739,35 +1747,39 @@
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+    <row r="17" spans="1:10" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="D17" s="24"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="26" t="s">
-        <v>33</v>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -1778,9 +1790,9 @@
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -1791,9 +1803,9 @@
       <c r="I20" s="2"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -1804,22 +1816,22 @@
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
@@ -1830,9 +1842,9 @@
       <c r="I23" s="2"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -1843,9 +1855,9 @@
       <c r="I24" s="2"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -1856,9 +1868,9 @@
       <c r="I25" s="2"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
@@ -1869,9 +1881,9 @@
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -1882,9 +1894,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -1895,9 +1907,9 @@
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
@@ -1908,9 +1920,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
@@ -1921,9 +1933,9 @@
       <c r="I30" s="2"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
@@ -1934,9 +1946,9 @@
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
@@ -1947,9 +1959,9 @@
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -1960,9 +1972,9 @@
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
@@ -1973,9 +1985,9 @@
       <c r="I34" s="2"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
@@ -1986,9 +1998,9 @@
       <c r="I35" s="2"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
@@ -1999,9 +2011,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="27" t="s">
-        <v>52</v>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
@@ -2012,9 +2024,9 @@
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="26" t="s">
-        <v>53</v>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -2025,9 +2037,9 @@
       <c r="I38" s="2"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
@@ -2038,9 +2050,9 @@
       <c r="I39" s="2"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
@@ -2051,9 +2063,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
@@ -2064,9 +2076,9 @@
       <c r="I41" s="2"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
@@ -2077,16 +2089,12 @@
       <c r="I42" s="2"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="120" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>60</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="24"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2094,12 +2102,16 @@
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>59</v>
+      </c>
       <c r="D44" s="24"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2107,9 +2119,9 @@
       <c r="I44" s="2"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
@@ -2120,9 +2132,9 @@
       <c r="I45" s="2"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -2133,9 +2145,9 @@
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -2146,9 +2158,9 @@
       <c r="I47" s="2"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
@@ -2159,9 +2171,9 @@
       <c r="I48" s="2"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="24"/>
@@ -2172,9 +2184,9 @@
       <c r="I49" s="2"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
@@ -2185,9 +2197,9 @@
       <c r="I50" s="2"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
@@ -2198,9 +2210,9 @@
       <c r="I51" s="2"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="24"/>
@@ -2211,9 +2223,9 @@
       <c r="I52" s="2"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="24"/>
@@ -2224,16 +2236,12 @@
       <c r="I53" s="2"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" ht="172.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>73</v>
-      </c>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
       <c r="D54" s="24"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2241,15 +2249,15 @@
       <c r="I54" s="2"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" ht="331.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="D55" s="24"/>
       <c r="F55" s="1"/>
@@ -2258,14 +2266,16 @@
       <c r="I55" s="2"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="320.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" s="24"/>
+        <v>74</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>75</v>
+      </c>
       <c r="D56" s="24"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2273,16 +2283,14 @@
       <c r="I56" s="2"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>81</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C57" s="24"/>
       <c r="D57" s="24"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2290,15 +2298,15 @@
       <c r="I57" s="2"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="30" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>80</v>
       </c>
       <c r="D58" s="24"/>
       <c r="F58" s="1"/>
@@ -2307,14 +2315,16 @@
       <c r="I58" s="2"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="1:10" ht="231" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C59" s="24"/>
+        <v>81</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="D59" s="24"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2322,11 +2332,13 @@
       <c r="I59" s="2"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="24"/>
+    <row r="60" spans="1:10" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>85</v>
+      </c>
       <c r="C60" s="24"/>
       <c r="D60" s="24"/>
       <c r="F60" s="1"/>
@@ -2335,9 +2347,9 @@
       <c r="I60" s="2"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="28" t="s">
-        <v>88</v>
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="31" t="s">
+        <v>86</v>
       </c>
       <c r="B61" s="24"/>
       <c r="C61" s="24"/>
@@ -2348,9 +2360,9 @@
       <c r="I61" s="2"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B62" s="24"/>
       <c r="C62" s="24"/>
@@ -2361,9 +2373,9 @@
       <c r="I62" s="2"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B63" s="24"/>
       <c r="C63" s="24"/>
@@ -2374,9 +2386,9 @@
       <c r="I63" s="2"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" s="24"/>
       <c r="C64" s="24"/>
@@ -2387,9 +2399,9 @@
       <c r="I64" s="2"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B65" s="24"/>
       <c r="C65" s="24"/>
@@ -2400,9 +2412,9 @@
       <c r="I65" s="2"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -2413,9 +2425,9 @@
       <c r="I66" s="2"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B67" s="24"/>
       <c r="C67" s="24"/>
@@ -2426,9 +2438,9 @@
       <c r="I67" s="2"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
@@ -2439,9 +2451,9 @@
       <c r="I68" s="2"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B69" s="24"/>
       <c r="C69" s="24"/>
@@ -2452,9 +2464,9 @@
       <c r="I69" s="2"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
@@ -2465,9 +2477,9 @@
       <c r="I70" s="2"/>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="31" t="s">
-        <v>98</v>
+    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
@@ -2478,9 +2490,9 @@
       <c r="I71" s="2"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="28" t="s">
-        <v>99</v>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="B72" s="24"/>
       <c r="C72" s="24"/>
@@ -2491,9 +2503,9 @@
       <c r="I72" s="2"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B73" s="24"/>
       <c r="C73" s="24"/>
@@ -2504,9 +2516,9 @@
       <c r="I73" s="2"/>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="31" t="s">
-        <v>101</v>
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="28" t="s">
+        <v>99</v>
       </c>
       <c r="B74" s="24"/>
       <c r="C74" s="24"/>
@@ -2517,9 +2529,9 @@
       <c r="I74" s="2"/>
       <c r="J74" s="3"/>
     </row>
-    <row r="75" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="28" t="s">
-        <v>102</v>
+    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="31" t="s">
+        <v>100</v>
       </c>
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
@@ -2530,9 +2542,9 @@
       <c r="I75" s="2"/>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="31" t="s">
-        <v>103</v>
+    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="28" t="s">
+        <v>101</v>
       </c>
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
@@ -2543,9 +2555,9 @@
       <c r="I76" s="2"/>
       <c r="J76" s="3"/>
     </row>
-    <row r="77" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="28" t="s">
-        <v>104</v>
+    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
@@ -2556,9 +2568,9 @@
       <c r="I77" s="2"/>
       <c r="J77" s="3"/>
     </row>
-    <row r="78" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
@@ -2569,9 +2581,9 @@
       <c r="I78" s="2"/>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B79" s="24"/>
       <c r="C79" s="24"/>
@@ -2582,9 +2594,9 @@
       <c r="I79" s="2"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
@@ -2595,9 +2607,9 @@
       <c r="I80" s="2"/>
       <c r="J80" s="3"/>
     </row>
-    <row r="81" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B81" s="24"/>
       <c r="C81" s="24"/>
@@ -2608,9 +2620,9 @@
       <c r="I81" s="2"/>
       <c r="J81" s="3"/>
     </row>
-    <row r="82" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="31" t="s">
-        <v>109</v>
+    <row r="82" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="28" t="s">
+        <v>107</v>
       </c>
       <c r="B82" s="24"/>
       <c r="C82" s="24"/>
@@ -2621,9 +2633,9 @@
       <c r="I82" s="2"/>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="28" t="s">
-        <v>110</v>
+    <row r="83" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="B83" s="24"/>
       <c r="C83" s="24"/>
@@ -2634,9 +2646,9 @@
       <c r="I83" s="2"/>
       <c r="J83" s="3"/>
     </row>
-    <row r="84" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B84" s="24"/>
       <c r="C84" s="24"/>
@@ -2647,9 +2659,9 @@
       <c r="I84" s="2"/>
       <c r="J84" s="3"/>
     </row>
-    <row r="85" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B85" s="24"/>
       <c r="C85" s="24"/>
@@ -2660,9 +2672,9 @@
       <c r="I85" s="2"/>
       <c r="J85" s="3"/>
     </row>
-    <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B86" s="24"/>
       <c r="C86" s="24"/>
@@ -2673,9 +2685,9 @@
       <c r="I86" s="2"/>
       <c r="J86" s="3"/>
     </row>
-    <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B87" s="24"/>
       <c r="C87" s="24"/>
@@ -2686,9 +2698,9 @@
       <c r="I87" s="2"/>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B88" s="24"/>
       <c r="C88" s="24"/>
@@ -2699,9 +2711,9 @@
       <c r="I88" s="2"/>
       <c r="J88" s="3"/>
     </row>
-    <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B89" s="24"/>
       <c r="C89" s="24"/>
@@ -2712,9 +2724,9 @@
       <c r="I89" s="2"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B90" s="24"/>
       <c r="C90" s="24"/>
@@ -2725,9 +2737,9 @@
       <c r="I90" s="2"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="32" t="s">
-        <v>118</v>
+    <row r="91" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="B91" s="24"/>
       <c r="C91" s="24"/>
@@ -2738,9 +2750,9 @@
       <c r="I91" s="2"/>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B92" s="24"/>
       <c r="C92" s="24"/>
@@ -2751,9 +2763,9 @@
       <c r="I92" s="2"/>
       <c r="J92" s="3"/>
     </row>
-    <row r="93" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B93" s="24"/>
       <c r="C93" s="24"/>
@@ -2764,9 +2776,9 @@
       <c r="I93" s="2"/>
       <c r="J93" s="3"/>
     </row>
-    <row r="94" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B94" s="24"/>
       <c r="C94" s="24"/>
@@ -2777,9 +2789,9 @@
       <c r="I94" s="2"/>
       <c r="J94" s="3"/>
     </row>
-    <row r="95" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B95" s="24"/>
       <c r="C95" s="24"/>
@@ -2790,9 +2802,9 @@
       <c r="I95" s="2"/>
       <c r="J95" s="3"/>
     </row>
-    <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B96" s="24"/>
       <c r="C96" s="24"/>
@@ -2803,9 +2815,9 @@
       <c r="I96" s="2"/>
       <c r="J96" s="3"/>
     </row>
-    <row r="97" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B97" s="24"/>
       <c r="C97" s="24"/>
@@ -2816,9 +2828,9 @@
       <c r="I97" s="2"/>
       <c r="J97" s="3"/>
     </row>
-    <row r="98" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B98" s="24"/>
       <c r="C98" s="24"/>
@@ -2829,9 +2841,9 @@
       <c r="I98" s="2"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="33" t="s">
-        <v>126</v>
+    <row r="99" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="B99" s="24"/>
       <c r="C99" s="24"/>
@@ -2842,9 +2854,9 @@
       <c r="I99" s="2"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="32" t="s">
-        <v>127</v>
+    <row r="100" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="33" t="s">
+        <v>125</v>
       </c>
       <c r="B100" s="24"/>
       <c r="C100" s="24"/>
@@ -2855,9 +2867,9 @@
       <c r="I100" s="2"/>
       <c r="J100" s="3"/>
     </row>
-    <row r="101" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B101" s="24"/>
       <c r="C101" s="24"/>
@@ -2868,9 +2880,9 @@
       <c r="I101" s="2"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="33" t="s">
-        <v>129</v>
+    <row r="102" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="32" t="s">
+        <v>127</v>
       </c>
       <c r="B102" s="24"/>
       <c r="C102" s="24"/>
@@ -2881,9 +2893,9 @@
       <c r="I102" s="2"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="32" t="s">
-        <v>130</v>
+    <row r="103" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="33" t="s">
+        <v>128</v>
       </c>
       <c r="B103" s="24"/>
       <c r="C103" s="24"/>
@@ -2894,9 +2906,9 @@
       <c r="I103" s="2"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
@@ -2907,9 +2919,9 @@
       <c r="I104" s="2"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B105" s="24"/>
       <c r="C105" s="24"/>
@@ -2920,496 +2932,509 @@
       <c r="I105" s="2"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B106" s="24"/>
       <c r="C106" s="24"/>
       <c r="D106" s="24"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="6"/>
-    </row>
-    <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="3"/>
+    </row>
+    <row r="107" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B107" s="24"/>
       <c r="C107" s="24"/>
       <c r="D107" s="24"/>
-    </row>
-    <row r="108" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="6"/>
+    </row>
+    <row r="108" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B108" s="24"/>
       <c r="C108" s="24"/>
       <c r="D108" s="24"/>
     </row>
-    <row r="109" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B109" s="24"/>
       <c r="C109" s="24"/>
       <c r="D109" s="24"/>
     </row>
-    <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B110" s="24"/>
       <c r="C110" s="24"/>
       <c r="D110" s="24"/>
     </row>
-    <row r="111" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B111" s="24"/>
       <c r="C111" s="24"/>
       <c r="D111" s="24"/>
     </row>
-    <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B112" s="24"/>
       <c r="C112" s="24"/>
       <c r="D112" s="24"/>
     </row>
-    <row r="113" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B113" s="24"/>
       <c r="C113" s="24"/>
       <c r="D113" s="24"/>
     </row>
-    <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B114" s="24"/>
       <c r="C114" s="24"/>
       <c r="D114" s="24"/>
     </row>
-    <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B115" s="24"/>
       <c r="C115" s="24"/>
       <c r="D115" s="24"/>
     </row>
-    <row r="116" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
       <c r="D116" s="24"/>
     </row>
-    <row r="117" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B117" s="24"/>
       <c r="C117" s="24"/>
       <c r="D117" s="24"/>
     </row>
-    <row r="118" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B118" s="24"/>
       <c r="C118" s="24"/>
       <c r="D118" s="24"/>
     </row>
-    <row r="119" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B119" s="24"/>
       <c r="C119" s="24"/>
       <c r="D119" s="24"/>
     </row>
-    <row r="120" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="34" t="s">
+    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B120" s="24"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="24"/>
+    </row>
+    <row r="121" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B121" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B120" s="25" t="s">
+      <c r="C121" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="C120" s="35" t="s">
+      <c r="D121" s="24"/>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="34" t="s">
         <v>149</v>
-      </c>
-      <c r="D120" s="24"/>
-    </row>
-    <row r="121" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="B121" s="24"/>
-      <c r="C121" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="D121" s="24"/>
-    </row>
-    <row r="122" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="34" t="s">
-        <v>151</v>
       </c>
       <c r="B122" s="24"/>
       <c r="C122" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D122" s="24"/>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B123" s="24"/>
+      <c r="C123" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D123" s="24"/>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="34" t="s">
         <v>151</v>
-      </c>
-      <c r="D122" s="24"/>
-    </row>
-    <row r="123" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="B123" s="24"/>
-      <c r="C123" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D123" s="24"/>
-    </row>
-    <row r="124" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="34" t="s">
-        <v>153</v>
       </c>
       <c r="B124" s="24"/>
       <c r="C124" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D124" s="24"/>
     </row>
-    <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B125" s="24"/>
       <c r="C125" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D125" s="24"/>
     </row>
-    <row r="126" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B126" s="24"/>
       <c r="C126" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D126" s="24"/>
     </row>
-    <row r="127" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B127" s="24"/>
       <c r="C127" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D127" s="24"/>
     </row>
-    <row r="128" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B128" s="24"/>
       <c r="C128" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D128" s="24"/>
     </row>
-    <row r="129" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B129" s="24"/>
       <c r="C129" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D129" s="24"/>
     </row>
-    <row r="130" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B130" s="24"/>
       <c r="C130" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D130" s="24"/>
     </row>
-    <row r="131" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B131" s="24"/>
       <c r="C131" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D131" s="24"/>
     </row>
-    <row r="132" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B132" s="24"/>
       <c r="C132" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D132" s="24"/>
     </row>
-    <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B133" s="24"/>
       <c r="C133" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D133" s="24"/>
     </row>
-    <row r="134" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B134" s="24"/>
       <c r="C134" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D134" s="24"/>
     </row>
-    <row r="135" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="B135" s="24"/>
+      <c r="C135" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D135" s="24"/>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B136" s="24"/>
+      <c r="C136" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="D136" s="24"/>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="34" t="s">
         <v>164</v>
-      </c>
-      <c r="B135" s="24"/>
-      <c r="C135" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="D135" s="24"/>
-    </row>
-    <row r="136" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="B136" s="24"/>
-      <c r="C136" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D136" s="24"/>
-    </row>
-    <row r="137" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="34" t="s">
-        <v>166</v>
       </c>
       <c r="B137" s="24"/>
       <c r="C137" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D137" s="24"/>
     </row>
-    <row r="138" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B138" s="24"/>
       <c r="C138" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D138" s="24"/>
     </row>
-    <row r="139" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B139" s="24"/>
       <c r="C139" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D139" s="24"/>
     </row>
-    <row r="140" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B140" s="24"/>
       <c r="C140" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D140" s="24"/>
     </row>
-    <row r="141" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B141" s="24"/>
       <c r="C141" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D141" s="24"/>
     </row>
-    <row r="142" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B142" s="24"/>
+      <c r="C142" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D142" s="24"/>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="B143" s="24"/>
+      <c r="C143" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="D143" s="24"/>
+    </row>
+    <row r="144" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="B142" s="24"/>
-      <c r="C142" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D142" s="24"/>
-    </row>
-    <row r="143" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="34" t="s">
+      <c r="B144" s="24"/>
+      <c r="C144" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D144" s="24"/>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="B143" s="24"/>
-      <c r="C143" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D143" s="24"/>
-    </row>
-    <row r="144" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="34" t="s">
+      <c r="B145" s="24"/>
+      <c r="C145" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D145" s="24"/>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="34" t="s">
         <v>173</v>
-      </c>
-      <c r="B144" s="24"/>
-      <c r="C144" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="D144" s="24"/>
-    </row>
-    <row r="145" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="B145" s="24"/>
-      <c r="C145" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D145" s="24"/>
-    </row>
-    <row r="146" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="34" t="s">
-        <v>175</v>
       </c>
       <c r="B146" s="24"/>
       <c r="C146" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D146" s="24"/>
     </row>
-    <row r="147" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B147" s="24"/>
       <c r="C147" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D147" s="24"/>
     </row>
-    <row r="148" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="34" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B148" s="24"/>
       <c r="C148" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D148" s="24"/>
     </row>
-    <row r="149" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B149" s="24"/>
       <c r="C149" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D149" s="24"/>
     </row>
-    <row r="150" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B150" s="24"/>
       <c r="C150" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D150" s="24"/>
     </row>
-    <row r="151" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B151" s="24"/>
       <c r="C151" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D151" s="24"/>
     </row>
-    <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="B152" s="24"/>
+      <c r="C152" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D152" s="24"/>
+    </row>
+    <row r="153" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B153" s="24"/>
+      <c r="C153" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="D153" s="24"/>
+    </row>
+    <row r="154" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="B152" s="24"/>
-      <c r="C152" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="D152" s="24"/>
-    </row>
-    <row r="153" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="37" t="s">
+      <c r="B154" s="24"/>
+      <c r="C154" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D154" s="24"/>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="38" t="s">
         <v>182</v>
-      </c>
-      <c r="B153" s="24"/>
-      <c r="C153" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D153" s="24"/>
-    </row>
-    <row r="154" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B154" s="24"/>
-      <c r="C154" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="D154" s="24"/>
-    </row>
-    <row r="155" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="34" t="s">
-        <v>184</v>
       </c>
       <c r="B155" s="24"/>
       <c r="C155" s="36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D155" s="24"/>
+    </row>
+    <row r="156" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="B156" s="24"/>
+      <c r="C156" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D156" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" location="United_States" xr:uid="{C3D40FAD-0EF1-4851-A69D-66AAF38D443D}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{62572206-46B5-4135-A74F-8DC12B1DFC8E}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{DA014289-02EC-425D-9D5B-0BF4ABEEFF65}"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://www.marinha.mil.br/secirm/psrm/ppgmar" xr:uid="{AFBDDCF0-E72E-4E7E-B4C9-A58CFFADC36F}"/>
-    <hyperlink ref="B59" r:id="rId5" display="https://www.unenvironment.org/nairobiconvention/comoros-towards-network-marine-protection" xr:uid="{A49A6E31-99B5-4F32-AFAD-D4EE967B6535}"/>
-    <hyperlink ref="B120" r:id="rId6" display="https://biodiversity.europa.eu/" xr:uid="{8D14DEB1-7D73-4BBB-9627-8C63E5B81A30}"/>
+    <hyperlink ref="E4" r:id="rId1" location="United_States"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.marinha.mil.br/secirm/psrm/ppgmar"/>
+    <hyperlink ref="B60" r:id="rId5" display="https://www.unenvironment.org/nairobiconvention/comoros-towards-network-marine-protection"/>
+    <hyperlink ref="B121" r:id="rId6" display="https://biodiversity.europa.eu/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
new logo, updated texts
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -33,26 +33,25 @@
 examining how this data are represented and used, this project will create a novel understanding of the
 materiality of science-policy interrelations in global environmental politics as well as develop the
 methodologies to do so. 
-&lt;br&gt;
+&lt;p&gt;
 This is crucial, because the capacities to develop and use data infrastructures are unequally distributed
 among countries and global initiatives for data sharing are significantly challenged by conflicting perceptions
 of who benefits from marine biodiversity research. Despite broad recognition of these challenges within natural
 science communities the political aspects of marine biodiversity data remain understudied. Academic debates
 tend to neglect the role of international politics in legitimising and authorising scientific concepts, data sources
 and criteria and how this influences national monitoring priorities.
-&lt;br&gt;
+&lt;p&gt;
 The central objective of MARIPOLDATA is to overcome these shortcomings by developing and
 applying a new multiscale methodology for grounding the analysis of science-policy interrelations in empirical
 research. An interdisciplinary team, led by the PI, collects and analyse data across different policy-levels
 and spatial scales by combining 1) ethnographic studies at intergovernmental negotiation sites with 2) a
 comparative analysis of national biodiversity monitoring policies and practices and 3) bibliometric and
 network analyses and oral history interviews for mapping marine biodiversity science.
-&lt;br&gt;&lt;/br&gt;
-This section informs about the bibliometric analysis of marine biodiversity sciences:
+&lt;p&gt;
 International scientific collaboration is essential to support global and regional efforts to protect marine biodiversity in areas within and beyond national jurisdiction. Several scientific programs and initiatives, such as the International Census of Marine Life Programme or the recently launched UN Decade of Ocean Science take the need to enhance scientific cooperation across regions into account to close data gaps, align research programs, and support conservation efforts. &lt;br&gt;
 Marine biodiversity research spans different spatial and temporal scales to assess global biodiversity loss patterns and is considered one of the most complex scientific fields to have emerged in recent decades [10]. As a big science, it ties together research teams, scientific infrastructures, laboratories, and equipment from different countries and regions of the world. While international scientific collaboration seems to be inherent to the marine biodiversity field, it is also highly encouraged by the United Nations Convention on the Law of the Sea (UNCLOS). &lt;br&gt;
-For more explanation of the methodological approach to researching marine biodiversity science bibliometrically, please refer to the following 
-&lt;p&gt;&lt;a href="https://www.sciencedirect.com/science/article/pii/S0308597X20309659"&gt;paper&lt;/a&gt;&lt;/p&gt;.</t>
+For more explanation of the methodological approach to researching marine biodiversity science bibliometrically, please refer to the  &lt;a href="https://www.sciencedirect.com/science/article/pii/S0308597X20309659"&gt;paper&lt;/a&gt; by Tolochko &amp; Vadrot (2021).
+&lt;p&gt;This section informs about the bibliometric analysis of marine biodiversity sciences.</t>
   </si>
   <si>
     <r>
@@ -61,33 +60,18 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t>In order to protect marine biodiversity and ensure that benefits are equally shared, the UN General
-Assembly has decided to develop a new legally binding treaty under the United Nations Convention on the
-Law of the Sea. Marine biodiversity data will play a central role: Firstly, in supporting intergovernmental
-efforts to identify, protect and monitor marine biodiversity. Secondly, in informing governments interested in
-particular aspects of marine biodiversity, including its economic use and its contribution to biosecurity. In
-examining how this data are represented and used, this project will create a novel understanding of the
-materiality of science-policy interrelations in global environmental politics as well as develop the
-methodologies to do so. 
-&lt;br&gt;
-This is crucial, because the capacities to develop and use data infrastructures are unequally distributed
-among countries and global initiatives for data sharing are significantly challenged by conflicting perceptions
-of who benefits from marine biodiversity research. Despite broad recognition of these challenges within natural
-science communities the political aspects of marine biodiversity data remain understudied. Academic debates
-tend to neglect the role of international politics in legitimising and authorising scientific concepts, data sources
-and criteria and how this influences national monitoring priorities.
-&lt;br&gt;
-The central objective of MARIPOLDATA is to overcome these shortcomings by developing and
-applying a new multiscale methodology for grounding the analysis of science-policy interrelations in empirical
-research. An interdisciplinary team, led by the PI, collects and analyse data across different policy-levels
-and spatial scales by combining 1) ethnographic studies at intergovernmental negotiation sites with 2) a
-comparative analysis of national biodiversity monitoring policies and practices and 3) bibliometric and
-network analyses and oral history interviews for mapping marine biodiversity science.
-&lt;br&gt;&lt;/br&gt;
-Over one hundred governments are currently negotiating a new legally binding instrument for the conservation and sustainable use of marine biological diversity in areas beyond national jurisdiction (BBNJ). The new agreement is to address four broad themes: marine genetic resources (MGRs); area-based management tools (ABMTs), including marine protected areas (MPAs); environmental impact assessments (EIAs); and capacity building and the transfer of marine technology (CB&amp;TT). 
-&lt;br&gt; 
-For an overview of the ongoing negotiations, please refer to this 
-&lt;p&gt;&lt;a hre</t>
+      <t xml:space="preserve">The Convention on the Law of the Sea (UNCLOS), which entered into force in 1994, established a 12
+mile territorial sea - meaning that states have sovereignty over this area and creating a 200 mile exclusive
+economic zone (EEZ) (Harrison, 2017; Rochette et al. 2014). However, a lack of regulation beyond this zone,
+continues to facilitate the uncontrolled pollution and extraction of natural resources from the oceans and
+undermines the establishment of MPAs (Vogler 2012). In order to address this challenge, the UN General
+Assembly developed an international legally binding instrument under UNCLOS on the conservation and
+sustainable use of marine biodiversity of areas beyond national jurisdiction (resolution 69/292 of 19 June
+2015).
+&lt;p&gt;
+Since 2018, over one hundred governments are negotiating a new legally binding instrument for the conservation and sustainable use of marine biological diversity in areas beyond national jurisdiction (BBNJ). The new agreement is to address four broad themes: marine genetic resources (MGRs); area-based management tools (ABMTs), including marine protected areas (MPAs); environmental impact assessments (EIAs); and capacity building and the transfer of marine technology (CB&amp;TT). 
+&lt;p&gt; 
+For an overview of the ongoing negotiations, please refer to the &lt;a </t>
     </r>
     <r>
       <rPr>
@@ -95,7 +79,7 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t>f="</t>
+      <t>href="</t>
     </r>
     <r>
       <rPr>
@@ -112,8 +96,8 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t>"&gt;paper&lt;/a&gt;&lt;/p&gt;.
-This section informs about the ongoing ethnographic work at the UN BBNJ negotiations:</t>
+      <t>"&gt;paper&lt;/a&gt; by Tessnow-von Wysocki &amp; Vadrot (2021).
+&lt;p&gt;This section informs about the ongoing ethnographic work at the UN BBNJ negotiations.&lt;/p&gt;</t>
     </r>
   </si>
   <si>
@@ -157,18 +141,9 @@
     </r>
   </si>
   <si>
-    <t>The BBNJ Working Group started meeting in 2006 and the EU has been a strong promotor of this political process since its beginning calling for the adoption of an UNCLOS 1A (Druel &amp; Gjerde, 2014; European Commission, 2019). Nevertheless, this early idea did not include MGRs and failed to reach a global consensus to sustain negotiations and therefore it took up an increased political interests only after 2009 (own interview, 2019). 
+    <t xml:space="preserve">The BBNJ Working Group started meeting in 2006 and the EU has been a strong promotor of this political process since its beginning calling for the adoption of an UNCLOS 1A (Druel &amp; Gjerde, 2014; European Commission, 2019). Nevertheless, this early idea did not include MGRs and failed to reach a global consensus to sustain negotiations and therefore it took up an increased political interests only after 2009 (own interview, 2019). 
  The EU represents a broad field of interested states in the negotiations that consistently negotiate under a common mandate. 
- MGRs
- The EU’s delegate diverted from the strict naming-naming-of-options method of negotiation and made a more logical argument based statement, emphasizing that the EU favours a “holistic approach” for MGRs. The statements focussed on operationalizing the provisions of the treaty on the sharing of information, scientific data, and knowledge and the building of research capacities. The EU delegate reiterated that the EU does not support addressing intellectual property rights under the new treaty (supported by the US, Switzerland, Norway, Holy See, Japan, The Republic of Korea, The Russian Federation and Australia). The EU also stated that fish or other biological commodities should not be addressed. It was noted that activities related to MGRs are in essence marine scientific research, which should not be hampered in any way. It was argued that the clearing house is a cross-cutting issue in itself and Anca Leroy rejecting a possible connection to Nagoya in the treaty text.
- ABMTs:
- The EU alongside Micronesia, Cameroon, New Zealand, and the High Seas Alliance favoured reference to traditional knowledge as an additional source of information but remained critical to the inclusion of economic and social factors in the identification of areas. The EU strongly supported the application of the precautionary principle, the ecosystem approach and a reference to best available science whereas the US, Singapore, Australia, Canada and Japan favoured the precautionary approach. It was explained that a lack of scientific knowledge should not justify taking no protecting measures. Furthermore, the EU supported the establishment of a connected network of MPAs. Proposals of ABMTs should be reviewed by a scientific/technical body and designated by a COP which would also possess the authority of the designated area.
- EIAs: 
- The EU as well as the Likeminded Latin American Countries, G-77/China, the African Group, P-SIDS, CARICOM and Canada supported the outlining the steps, albeit in a little detailed manner, for conducting an EIA in the treaty as opposed to establish the process later on. The EU supported requiring a description of planned activities as well as a description of reasonable alternatives in an EIA. Under descriptions of impacts, the EU, alongside P-SIDS, the US, India, Norway, Indonesia, Canada and the African Group supported describing effects, including cumulative and transboundary impacts. The EU furthermore made a reference to the CBD for detailed guidelines on EIAs and noted that EBSAs can be helpful to determine the location and characterization of the ecosystem. Finally, the EU, with many others, argued that compliance should be taken up under cross-cutting issues and favoured an activity-based approach to defining the threshold for an EIA.
- CBTT:
- On CBTT, the EU noted that the list of types and modalities is too long. Nevertheless, the EU agreed with the African Group, the G-77/CHINA, CARICOM, the Like-Minded Latin American Countries, and P-SIDS that funding should be both voluntary and mandatory, with the EU underlining that mandatory funding be restricted to institutional and clearinghouse mechanism costs. On sources, the EU called for including national funding sources, and P-SIDS welcomed the inclusion of innovative funding sources. The EU proposed that a CHM can be established and supported the definition of functions and goals of a clearinghouse mechanism.
- Cross-Cutting Issues:
- Under Cross-Cutting Issues, a decision-making body or forum was discussed. The EU alongside the G-77/China, AOSIS, the African Group, Canada, Iceland and others supported establishing a COP under the implementing agreement and the EU noted that a provision on the first meeting of the COP should be explicitly included in the agreement. Concerning formulating the form and functions of the body, it was noted that it should be adequate to achieve the objectives, suggesting distinguishing between institutional and substantial functions. The EU supported the establishment of a scientific/technical body, preferring a scientific body and calling for flexibility to allow additional tasks to be mandated by the COP. The EU suggested the development of a pool of independent scientific experts, but also using expertise from existing arrangements. The EU argued that the functioning of a CHM can be discussed by the following COP. Where the G-77/China, the African Group, P-SIDS an others called for the inclusion of common heritage of humankind as a general principle, the EU but remained open to the common heritage of mankind principle, clarifying that principles that need to be stated in general provisions and those which should be operationalized in special sections are separated. Concerning definitions, the EU referred to UNCLOS and CBD.</t>
+</t>
   </si>
   <si>
     <t>brazil</t>
@@ -203,18 +178,9 @@
     </r>
   </si>
   <si>
-    <t>Within the UN framework, Brazil forms part of the Latin American and Carribean group of states but during the second Intergovernmental Conference (IGC 2) it negotiated through the group of Likeminded Latin American Countries. Because during IGC 1 Brazil and other Latin American countries still stated their individual preferences, it is concluded that the Latin American and likeminded Group formed particularly for the BBNJ process between IGC 1 and 2. The group of Like-Minded Latin American Countries consisted of Argentina, Brazil, Colombia, Costa Rica, Ecuador, El Salvador, Guatemala, Honduras, Mexico, Panama, Paraguay, Peru, Dominican Republic and Uruguay.
- Brazil spoke for the Like-Minded Latin American Countries group on Marine Genetic Resources (MGRs); Argentina on Area Based Management Tools (ABMTs) including Marine Protected Areas (MPAs); Uruguay on Environmental Impact Assessments (EIAs); Honduras on Capacity Building and Technology Transfer (CBTT) and Colombia on Cross-Cutting Issues. 
- MGRs
- In IGC 2 Brazil acted through the Likeminded Latin American Countries. The Brazilian Delegate Barbara Boechat was the spokesperson on behalf of the Group on the topic of MGRs. On MGRs, Brazil made clear that the Latin American and Liked-Minded Countries group preferred an option including the sharing of both monetary and non-monetary benefits, noting that only “voluntary benefits” is not workable. Brazil also argued that the principle of “common heritage of mankind” should be included in the section concerning the governing principles of benefit sharing not only for MGRs but for the whole treaty. Concerning the objectives and technicalities of benefit sharing modalities, Brazil stated on behalf of Like-Minded Latin American Countries and supported by the Republic Of Korea, that an overarching section on objectives including principles and approaches including a provision on a strong Clearing-House Mechanism (CHM) is preferable. On behalf of the Like-Minded Latin American Countries, Brazil supported the development of a non-exhaustive list of benefits within the treaty, as opposed to a list being developed at a later stage as well as the inclusion of monitoring measures by the CHM.
- ABMTs:
- On the identification of areas, Argentina on behalf of the Likeminded Latin American Countries alongside the G-77/China, Caricom, Sri Lanka, The African Group, Singapore and the High Seas Alliances supported a non-exhaustive list of standards and criteria for the identification of areas. On the designation of ABMTs including MPAs, the Likeminded Latin American Countries Group favoured that a decision making body can decide on the designation of all ABMTs. Furthermore, the Like-Minded Latin American Countries recognizes that consultation with concerned states, including adjacent coastal states is important. Uruguay further made a statement in relation to the inclusion of the EBSAs for the designation of ABMTs. 
- EIAs: 
- Uruguay on behalf of the Likeminded Latin American Countries and supported by G-77/China, the African Group, EU, P-SIDS, CARICOM and Canada argued against postponing the development of the EIA process and in favour of outlining the steps for conducting an EIA in the treaty. Uruguay supported that the content of an EIA should be described as detailed as possible including the determination of whether an EIA is needed. On the activities that need an EIA, The Like-Minded Latin American Countries, supported by the US, Norway, Australia, New Zealand and India, preferred that states parties assess whether they activities cause substantial pollution. On cumulative impacts, the Like-Minded Latin American Countries alongside the EU, Japan and Norway favoured also considering these impacts. Concerning the monitoring and review process, the Likeminded Latin American Countries group argued that these provisions should be moved to the general section. 
- CBTT:
- On CBTT, Honduras on behalf of the Like-Minded Latin American Countries supported - alongside the G-77/CHINA, CARICOM, AOSIS, NEW ZEALAND and INDIA - the inclusion of a list of CBTT activities and an outline of the modalities in the body of the treaty. Concerning the possible development of a clearinghouse mechanism, the Like-Minded Latin American Countries supported setting out the functions of a clearinghouse mechanism, however noting that this issue is cross-cutting and should be included in a general section. On the discussion of funding types, the group of Like-Minded Latin American Countries alongside the African Group, the G-77/China, the EU, CARICOM and the P-SIDS agreed that funding should be both voluntary and mandatory (however the EU noting that mandatory funding should be restricted to institutional and clearinghouse mechanism costs).
- Cross-Cutting Issues:
- On Cross-Cutting Issues, Colombia on behalf of the Like-Minded Latin American Countries stated that the group supports the establishment of a Conference of Parties as a decision-making body while asking to clarify the functions and the composition of the body. Furthermore, the Group supports the establishment of a secretariat and shows flexibility on where such a body would reside. Interestingly, the Like-Minded Latin American Countries alongside the African Group suggested removing references to high seas freedoms under the “General Principles and Approaches” section.</t>
+    <t xml:space="preserve">Within the UN framework, Brazil forms part of the Latin American and Carribean group of states but during the second Intergovernmental Conference (IGC 2) it negotiated through the group of Likeminded Latin American Countries. Because during IGC 1 Brazil and other Latin American countries still stated their individual preferences, it is concluded that the Latin American and likeminded Group formed particularly for the BBNJ process between IGC 1 and 2. The group of Like-Minded Latin American Countries consisted of Argentina, Brazil, Colombia, Costa Rica, Ecuador, El Salvador, Guatemala, Honduras, Mexico, Panama, Paraguay, Peru, Dominican Republic and Uruguay.
+Brazil spoke for the Like-Minded Latin American Countries group on Marine Genetic Resources (MGRs); Argentina on Area Based Management Tools (ABMTs) including Marine Protected Areas (MPAs); Uruguay on Environmental Impact Assessments (EIAs); Honduras on Capacity Building and Technology Transfer (CBTT) and Colombia on Cross-Cutting Issues. 
+ </t>
   </si>
   <si>
     <t>algeria</t>
@@ -461,14 +427,27 @@
     <t>holy see</t>
   </si>
   <si>
-    <t xml:space="preserve">The Holy See 
-The Holy See is the seat of the episcopal jurisdiction and the central government of the Catholic Church.
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The Holy See is the seat of the episcopal jurisdiction and the central government of the Catholic Church.
 Vatican City, within the territory of the Holy See, is a landlocked sovereign city-state located within the city of Rome, Italy and the headquarters of the Roman Catholic Church. It can be considered the world's smallest independent 'country' with a population of about 800 people and an area of 0.44 km² (0.17 sq mi) .
-https://www.nationsonline.org/oneworld/vatican.htm
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://www.nationsonline.org/oneworld/vatican.htm</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">
   https://holyseemission.org/contents//statements/5b9036cf0988a.php
   https://holyseemission.org/contents//newsletters/5bbe779a22936.php 
   https://enb.iisd.org/vol25/enb25195e.html
 </t>
+    </r>
   </si>
   <si>
     <t>The Holy See has been involved in the BBNJ process from the beginning of the Ad Hoc Open Ended Working groups in 2006, emphasizing the need for the protection of the environment . Susan Whelan is identified as serving the Holy See Mission as a legal expert following the UN Convention on the Law of the Sea contributing to an active role of Holy See in the BBNJ negotiations . Political positions mentioned by the delegation During the negotiations, the Holy See supported a hybrid approach (Kraabel, 2020). As regards the Holy See’s position during IGC2, they proposed two general provisions: a general stipulation of all activities not regulated by the ILBI; and a stipulation for MSR . Kraabel, K. (2020). Institutional arrangements in a BBNJ treaty: Implications for Arctic marine science. Marine Policy, 103807. doi:10.1016/j.marpol.2019.103807</t>
@@ -496,32 +475,33 @@
     <t>australia</t>
   </si>
   <si>
-    <t xml:space="preserve">Australia
-Australia’s marine estate is - with 13.86 km² - the 3rd largsest in the world. Australian waters include the great barrier reef - the largest reef system in the world- and Antarctic waters. 
+    <t xml:space="preserve">Australia’s marine estate is - with 13.86 km² - the 3rd largsest in the world. Australian waters include the great barrier reef - the largest reef system in the world- and Antarctic waters. 
 Australia has, as world leader in the management, conservation and sustainable use of the marine environment, an active presence and participation in international marine fora to promote Australia's interests by ensuring effective and complementary approaches to marine conservation on a regional and global level.
 The Department of Agriculture, Water and the Environment undertakes efforts in the region, including the common maritime boundaries in the Timor, Arafura and Coral Seas and the Torres Strait, and countries in the Indian Ocean, South East Asia and the Pacific. Measures aim to address transboundary marine conservation and environmental issues through informal discussions, cooperative programs, knowledge and skill-sharing with counterpart agencies, and formal agreements or legally binding instruments, recognizing that resources are shared and that sustainable use and successful biodiversity conservation measures can only be achieved through cooperation at a regional level. 
 Australia engages on the regional level through the Secretariat of the Pacific Regional Environment Programme (SPREP), Pacific Ocean Litter Project, The Coral Triangle Initiative for Coral Reefs, Fisheries and Food Security (CTI-CFF), Enhancing Pacific Ocean Governance (EPOG), Arafura and Timor Seas Ecosystems Action (ATSEA), Torres Strait Treaty Environmental Management Committee, Australia - France-New Caledonia Coral Sea Transboundary Collaboration, as well as in Regional Fisheries Management Organisations (RFMOs).
 Marine biodiversity beyond national jurisdiction
 Australia is actively engaged in negotiations for a new treaty under the United Nations Convention on the Law of the Sea (UNCLOS) on the conservation and sustainable use of marine biodiversity of areas beyond national jurisdiction (BBNJ).
+&lt;p&gt;
 National Science Institutions
 Established in 1972, the Australian Institute of Marine Science (AIMS) is Australia’s tropical marine research agency, providing large-scale, long-term and world-class research. It is committed to undertaking research that addresses real needs and provides impartial, authoritative advice, and that supports both the protection and sustainable use of our marine heritage, now and into the future.
 These aims are achieved through innovative scientific and technological research, and with the help of our people, industry and research partnerships, infrastructure, and comprehensive data sets, including:
-•        conducting strategic and applied research into marine life, from microbes to whole-of-ecosystems, and the processes that sustain them
-•        monitoring the condition and trends in the health of the marine environment
-•        building models and decision-support tools to assist interpretation of the data collected
-•        developing a broad spectrum of enabling technologies, from molecular sciences to ocean technologies.
+&lt;br&gt; •        conducting strategic and applied research into marine life, from microbes to whole-of-ecosystems, and the processes that sustain them
+&lt;br&gt; •        monitoring the condition and trends in the health of the marine environment
+&lt;br&gt; •        building models and decision-support tools to assist interpretation of the data collected
+&lt;br&gt; •        developing a broad spectrum of enabling technologies, from molecular sciences to ocean technologies.
 The Institute has 2 research vessels that go out at sea to undertake marine scientific research once a year. The AIMS Data Catalogue contains descriptions of data which allows others, including researchers, to identify potential data of use to them. Data can then be downloaded (if available) or requested. Access to some data will be via legal data agreement. See acces to the data catalougue here: https://apps.aims.gov.au/metadata/search 
 Journal publications of AIMS scientists are accessible in the AISM publication database: https://epubs.aims.gov.au/handle/11068/1
 Souce: https://www.aims.gov.au/docs/about/about.html
-o        Another renowned institution is the Commonwealth Scientific and Industrial Research Organisation (CSIRO), where environmental issues are dealt with alongside many other research areas. Overall, CSIRO has 5000 experts based in 59 centres, extensive local and international networks. With more than 1800 patents, we are Australia’s largest patent holder, holding an ever-increasing wealth of intellectual property is a vast source of commercial opportunity and has already resulted in more than 150 spin-off companies. Their research on environment includes Atmosphere &amp; climate , Circular Economy and Waste Management , Biodiversity, Extreme events , Land management , Oceans &amp; coasts and Water.
+&lt;p&gt;
+Another renowned institution is the Commonwealth Scientific and Industrial Research Organisation (CSIRO), where environmental issues are dealt with alongside many other research areas. Overall, CSIRO has 5000 experts based in 59 centres, extensive local and international networks. With more than 1800 patents, we are Australia’s largest patent holder, holding an ever-increasing wealth of intellectual property is a vast source of commercial opportunity and has already resulted in more than 150 spin-off companies. Their research on environment includes Atmosphere &amp; climate , Circular Economy and Waste Management , Biodiversity, Extreme events , Land management , Oceans &amp; coasts and Water.
 The Centre for Southern Hemisphere Oceans Research brings together researchers from Australia and China to further scientific understanding of the southern hemisphere oceans and their role in global and regional climate.
-•        Oceans and climate 
-o        Southern Oceans Research 
-o        Climate change information 
-o        Asia-Pacific climate science 
-o        Bluelink ocean forecasting 
-o        The Antarctic 
-o        Sea-level rise planning 
+&lt;br&gt; •         Oceans and climate 
+&lt;br&gt; •         Southern Oceans Research 
+&lt;br&gt; •         Climate change information 
+&lt;br&gt; •         Asia-Pacific climate science 
+&lt;br&gt; •         Bluelink ocean forecasting 
+&lt;br&gt; •         The Antarctic 
+&lt;br&gt; •         Sea-level rise planning 
 Most recent scientific findings regarding marine biodiversity can be found in a) the Oceans book, produced by CSIRO Publishing, providing a brief, accessible description of some of the key features of Australia’s marine estate, overviews of some areas where primary marine activities are supported by research, and some predictions of what marine research might look like in the near future; and b) the biodiversity book. Books are accessible here: https://www.csiro.au/en/Showcase/Oceans ;  https://www.csiro.au/en/Research/Environment/Biodiversity/Biodiversity-book/About 
 Source: https://www.csiro.au/en/About/We-are-CSIRO 
 https://www.csiro.au/en/Showcase/Oceans 
@@ -532,27 +512,27 @@
     <t>bangladesh</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Realizing the importance of ocean, the University of Chittagong has started marine science education and research by establishing the department of Marine Biology in 1971. In 2006, the department was renamed as the Institute of Marine Sciences and Fisheries (IMSF) to accommodate additional academic scope.
+    <t xml:space="preserve">Realizing the importance of ocean, the University of Chittagong has started marine science education and research by establishing the department of Marine Biology in 1971. In 2006, the department was renamed as the Institute of Marine Sciences and Fisheries (IMSF) to accommodate additional academic scope.
 Academic degrees offered at the IMSF are: BSc (Hon's) degrees in three subjects including Fisheries, Marine Science and Oceanography, and MSc degrees in six subjects including Fisheries, Oceanography, Aquaculture, Environmental Pollution and Management, Microbiology and Post-harvest Technology, and Fish and Shrimp Nutrition. It also offers research degrees (MPhil and PhD) and provides expert services in marine affairs to the government of Bangladesh, UN agencies, development partners, entrepreneurs, NGOs, and more. 
 More than 750 theses and dissertations have been completed at IMSF spanning a broad range of disciplines such as ecology, planktology, fisheries, aquaculture, oceanography, pollution, microbiology, climate science, geoinformatics, coastal zone and resource management, and biodiversity conservation of the northern Bay of Bengal and adjacent coastal/riverine ecosystems. This constitutes major portion of oceanographic, marine biological, fisheries and mariculture research findings in Bangladesh. 
 The Second International Indian Ocean Expedition (IIOE-2), on collaborative research from coastal environments to the deep sea over the period 2015-2020, aims to reveal new information on the Indian Ocean, to enhance our understanding to predict climate change impacts, pollution status, marine biogeochemical cycles, fisheries habitat, and sustainable management of resources (e.g. fisheries, petroleum, eco-tourism, and green energy), and ecosystem functions to strengthen economic and scientific competiveness of the Indian Ocean rim countries. 
+&lt;p&gt;
 The IIOE-2 includes:: 
-•        developing facility and enhancing national capacity on oceanographic research and application
-•        enhance capability of the young and early career scientists
-•        development of ocean observation and forecasting infrastructure
-•        ocean data management, archival, analysis and modeling capacities
-•        impact study of extreme events and monsoon variability on ecosystems and socio-economics
-•        monitoring change in ocean environments: warming, sea-level rise, deoxygenation, acidification, erosion/accretion, vegetation cover 
-•        physical and biological processes, biogeochemistry and ecology of the Bay of Bengal
-•        oil, gas and mineral resources exploration and exploitation
-•        factors that influence the dispersal of marine organisms
-•        food security and sustainable marine fisheries management
-•        safe navigation and fishing operation by fishermen
-•        sustainable blue growth activities
-•        renewable ocean energy
-•        climate change mitigation and adaptation planning
-•        outreach, participatory dissemination, awareness campaign, etc.
+&lt;br&gt; •         developing facility and enhancing national capacity on oceanographic research and application
+&lt;br&gt; •         enhance capability of the young and early career scientists
+&lt;br&gt; •         development of ocean observation and forecasting infrastructure
+&lt;br&gt; •         ocean data management, archival, analysis and modeling capacities
+&lt;br&gt; •         impact study of extreme events and monsoon variability on ecosystems and socio-economics
+&lt;br&gt; •         monitoring change in ocean environments: warming, sea-level rise, deoxygenation, acidification, erosion/accretion, vegetation cover 
+&lt;br&gt; •         physical and biological processes, biogeochemistry and ecology of the Bay of Bengal
+&lt;br&gt; •         oil, gas and mineral resources exploration and exploitation
+&lt;br&gt; •         factors that influence the dispersal of marine organisms
+&lt;br&gt; •         food security and sustainable marine fisheries management
+&lt;br&gt; •         safe navigation and fishing operation by fishermen
+&lt;br&gt; •         sustainable blue growth activities
+&lt;br&gt; •         renewable ocean energy
+&lt;br&gt; •         climate change mitigation and adaptation planning
+&lt;br&gt; •         outreach, participatory dissemination, awareness campaign, etc.
 source: https://incois.gov.in/IIOE-2/Bangladesh.jsp 
 </t>
   </si>
@@ -563,13 +543,13 @@
     <t>canada</t>
   </si>
   <si>
-    <t xml:space="preserve">Canada
-Canada is one of the Arctic coastal States, together with Norway, Denmark Greenland, Russian Federation and the United States. Canada is part of the Central Arctic Ocean Fisheries Agreement (CAOFA). The CAO includes portions of the Exclusive Economic Zones (EEZ) of Canada, Norway, Denmark/Greenland, and Russia (De Lucia, 2019).
-Science 
+    <t xml:space="preserve">Canada is one of the Arctic coastal States, together with Norway, Denmark Greenland, Russian Federation and the United States. Canada is part of the Central Arctic Ocean Fisheries Agreement (CAOFA). The CAO includes portions of the Exclusive Economic Zones (EEZ) of Canada, Norway, Denmark/Greenland, and Russia (De Lucia, 2019).
+&lt;p&gt;
 The Department of Fisheries and Oceans Canada (DFO) is the federal lead for safeguarding Canada’s waters and managing its fisheries, oceans and freshwater resources. Active in innovation in areas such as aquaculture and biotechnology, healthy and sustainable aquatic ecosystems are undertaken through habitat protection and sound science.
 DFO Science operates in over 17 DFO research institutes, laboratories, experimental centres and offices located in 7 regions across the country. The full list is available at: https://www.dfo-mpo.gc.ca/science/regions/index-eng.htm 
-Topics include Ocean and Climate Change Science, Oceanograohic activities, data managemet and modelling on national and regional levels. Research and monitoring provide advice on Canada's fisheries management, marine protected areas, species at risk, small craft harbours and maritime safety and security.
+Topics include Ocean and Climate Change Science, Oceanograohic activities, data managemet and modelling on national and regional levels. Research and monitoring provide advice on Canada's fisheries management, marine protected areas, species at risk, small craft harbours and maritime safety and security. 
 Oceanographic activities include observation of ocean and fresh water physical, chemical and biological conditions (e.g. tides, ocean currents, pH, salinity, temperature, ocean colour, phytoplankton, etc.) and the generation of models to assist in responding to emergencies (oil spills) and in evaluating the status of ecosystems. https://www.dfo-mpo.gc.ca/science/oceanography-oceanographie/activities/index-eng.html 
+&lt;p&gt;
 Data collected through departmental regional and zonal programs and from foreign sources, are assembled, processed and disseminated through Science and Data Centres operating in all regions. The database provides real-time/near real-time and historical ocean monitoring data and maintains archives of in-situ physical, chemical, and biological properties. See: http://www.isdm-gdsi.gc.ca/isdm-gdsi/index-eng.html
 Ocean models are based on ocean observations collected by earth observation satellites and direct measurement of conditions such as temperature, salinity, currents and wave heights. The computer-generated ocean models represent an ocean, or a region within an ocean, in three dimensions and depict its evolution over time. The connection between the atmosphere and the state of the ocean is accounted for by also including atmospheric data including wind stress, precipitation, evaporation, and cloud coverage. 
 With the increasing recognition that accurate ocean forecast models need to be "coupled models" that couple or incorporate information on atmospheric, ice, and ocean conditions, the model can be run to predict various aspects of ocean conditions which can then be used for operational oceanography, emergency preparedness planning, and to determine health of the oceans.
@@ -1319,6 +1299,9 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1327,9 +1310,6 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -3177,7 +3157,7 @@
       <c r="A55" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="15" t="s">
@@ -3243,7 +3223,7 @@
       <c r="A57" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C57" s="2"/>
@@ -3274,7 +3254,7 @@
       <c r="A58" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C58" s="15" t="s">
@@ -3307,7 +3287,7 @@
       <c r="A59" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="17" t="s">
         <v>81</v>
       </c>
       <c r="C59" s="15" t="s">
@@ -3691,7 +3671,7 @@
       <c r="Y71" s="2"/>
     </row>
     <row r="72">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="18" t="s">
         <v>98</v>
       </c>
       <c r="B72" s="2"/>
@@ -3778,7 +3758,7 @@
       <c r="Y74" s="2"/>
     </row>
     <row r="75">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="18" t="s">
         <v>101</v>
       </c>
       <c r="B75" s="2"/>
@@ -3836,7 +3816,7 @@
       <c r="Y76" s="2"/>
     </row>
     <row r="77">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="18" t="s">
         <v>103</v>
       </c>
       <c r="B77" s="2"/>
@@ -4010,7 +3990,7 @@
       <c r="Y82" s="2"/>
     </row>
     <row r="83">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="18" t="s">
         <v>109</v>
       </c>
       <c r="B83" s="2"/>
@@ -4126,7 +4106,7 @@
       <c r="Y86" s="2"/>
     </row>
     <row r="87">
-      <c r="A87" s="18" t="s">
+      <c r="A87" s="19" t="s">
         <v>113</v>
       </c>
       <c r="B87" s="2"/>
@@ -4155,7 +4135,7 @@
       <c r="Y87" s="2"/>
     </row>
     <row r="88">
-      <c r="A88" s="18" t="s">
+      <c r="A88" s="19" t="s">
         <v>114</v>
       </c>
       <c r="B88" s="2"/>
@@ -4184,7 +4164,7 @@
       <c r="Y88" s="2"/>
     </row>
     <row r="89">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B89" s="2"/>
@@ -4213,7 +4193,7 @@
       <c r="Y89" s="2"/>
     </row>
     <row r="90">
-      <c r="A90" s="18" t="s">
+      <c r="A90" s="19" t="s">
         <v>116</v>
       </c>
       <c r="B90" s="2"/>
@@ -4271,7 +4251,7 @@
       <c r="Y91" s="2"/>
     </row>
     <row r="92">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="20" t="s">
         <v>118</v>
       </c>
       <c r="B92" s="11" t="s">
@@ -4301,7 +4281,7 @@
       <c r="Y92" s="2"/>
     </row>
     <row r="93">
-      <c r="A93" s="19" t="s">
+      <c r="A93" s="20" t="s">
         <v>121</v>
       </c>
       <c r="B93" s="2"/>
@@ -4330,7 +4310,7 @@
       <c r="Y93" s="2"/>
     </row>
     <row r="94">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="20" t="s">
         <v>122</v>
       </c>
       <c r="B94" s="2"/>
@@ -4359,7 +4339,7 @@
       <c r="Y94" s="2"/>
     </row>
     <row r="95">
-      <c r="A95" s="19" t="s">
+      <c r="A95" s="20" t="s">
         <v>123</v>
       </c>
       <c r="B95" s="11" t="s">
@@ -4392,13 +4372,13 @@
       <c r="Y95" s="2"/>
     </row>
     <row r="96">
-      <c r="A96" s="19" t="s">
+      <c r="A96" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="C96" s="17" t="s">
         <v>128</v>
       </c>
       <c r="D96" s="2"/>
@@ -4425,7 +4405,7 @@
       <c r="Y96" s="2"/>
     </row>
     <row r="97">
-      <c r="A97" s="19" t="s">
+      <c r="A97" s="20" t="s">
         <v>129</v>
       </c>
       <c r="B97" s="2"/>
@@ -4454,7 +4434,7 @@
       <c r="Y97" s="2"/>
     </row>
     <row r="98">
-      <c r="A98" s="19" t="s">
+      <c r="A98" s="20" t="s">
         <v>130</v>
       </c>
       <c r="B98" s="2"/>
@@ -4512,7 +4492,7 @@
       <c r="Y99" s="2"/>
     </row>
     <row r="100">
-      <c r="A100" s="19" t="s">
+      <c r="A100" s="20" t="s">
         <v>132</v>
       </c>
       <c r="B100" s="2"/>
@@ -4541,13 +4521,13 @@
       <c r="Y100" s="2"/>
     </row>
     <row r="101">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B101" s="20" t="s">
+      <c r="B101" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C101" s="17" t="s">
         <v>135</v>
       </c>
       <c r="D101" s="2"/>
@@ -4574,7 +4554,7 @@
       <c r="Y101" s="2"/>
     </row>
     <row r="102">
-      <c r="A102" s="19" t="s">
+      <c r="A102" s="20" t="s">
         <v>136</v>
       </c>
       <c r="B102" s="2"/>
@@ -4603,7 +4583,7 @@
       <c r="Y102" s="2"/>
     </row>
     <row r="103">
-      <c r="A103" s="19" t="s">
+      <c r="A103" s="20" t="s">
         <v>137</v>
       </c>
       <c r="B103" s="2"/>
@@ -4632,13 +4612,13 @@
       <c r="Y103" s="2"/>
     </row>
     <row r="104">
-      <c r="A104" s="19" t="s">
+      <c r="A104" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B104" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C104" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D104" s="2"/>
@@ -4665,7 +4645,7 @@
       <c r="Y104" s="2"/>
     </row>
     <row r="105">
-      <c r="A105" s="19" t="s">
+      <c r="A105" s="20" t="s">
         <v>141</v>
       </c>
       <c r="B105" s="2"/>
@@ -4694,13 +4674,13 @@
       <c r="Y105" s="2"/>
     </row>
     <row r="106">
-      <c r="A106" s="19" t="s">
+      <c r="A106" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B106" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="17" t="s">
         <v>144</v>
       </c>
       <c r="D106" s="2"/>
@@ -4727,13 +4707,13 @@
       <c r="Y106" s="2"/>
     </row>
     <row r="107">
-      <c r="A107" s="19" t="s">
+      <c r="A107" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B107" s="20" t="s">
+      <c r="B107" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C107" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D107" s="2"/>
@@ -4760,13 +4740,13 @@
       <c r="Y107" s="2"/>
     </row>
     <row r="108">
-      <c r="A108" s="19" t="s">
+      <c r="A108" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B108" s="20" t="s">
+      <c r="B108" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="C108" s="20" t="s">
+      <c r="C108" s="17" t="s">
         <v>150</v>
       </c>
       <c r="D108" s="2"/>
@@ -4793,7 +4773,7 @@
       <c r="Y108" s="2"/>
     </row>
     <row r="109">
-      <c r="A109" s="19" t="s">
+      <c r="A109" s="20" t="s">
         <v>151</v>
       </c>
       <c r="B109" s="2"/>
@@ -4822,13 +4802,13 @@
       <c r="Y109" s="2"/>
     </row>
     <row r="110">
-      <c r="A110" s="19" t="s">
+      <c r="A110" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C110" s="17" t="s">
         <v>154</v>
       </c>
       <c r="D110" s="2"/>
@@ -4855,13 +4835,13 @@
       <c r="Y110" s="2"/>
     </row>
     <row r="111">
-      <c r="A111" s="19" t="s">
+      <c r="A111" s="20" t="s">
         <v>155</v>
       </c>
       <c r="B111" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="17" t="s">
         <v>157</v>
       </c>
       <c r="D111" s="2"/>
@@ -4888,7 +4868,7 @@
       <c r="Y111" s="2"/>
     </row>
     <row r="112">
-      <c r="A112" s="19" t="s">
+      <c r="A112" s="20" t="s">
         <v>158</v>
       </c>
       <c r="B112" s="2"/>
@@ -4917,7 +4897,7 @@
       <c r="Y112" s="2"/>
     </row>
     <row r="113">
-      <c r="A113" s="19" t="s">
+      <c r="A113" s="20" t="s">
         <v>159</v>
       </c>
       <c r="B113" s="2"/>
@@ -4946,7 +4926,7 @@
       <c r="Y113" s="2"/>
     </row>
     <row r="114">
-      <c r="A114" s="19" t="s">
+      <c r="A114" s="20" t="s">
         <v>160</v>
       </c>
       <c r="B114" s="2"/>
@@ -4975,13 +4955,13 @@
       <c r="Y114" s="2"/>
     </row>
     <row r="115">
-      <c r="A115" s="19" t="s">
+      <c r="A115" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="20" t="s">
+      <c r="B115" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C115" s="20" t="s">
+      <c r="C115" s="17" t="s">
         <v>163</v>
       </c>
       <c r="D115" s="2"/>
@@ -5124,13 +5104,13 @@
       <c r="Y119" s="2"/>
     </row>
     <row r="120">
-      <c r="A120" s="19" t="s">
+      <c r="A120" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B120" s="20" t="s">
+      <c r="B120" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="C120" s="20" t="s">
+      <c r="C120" s="17" t="s">
         <v>170</v>
       </c>
       <c r="D120" s="2"/>
@@ -30451,9 +30431,10 @@
     <hyperlink r:id="rId3" ref="B5"/>
     <hyperlink r:id="rId4" ref="B6"/>
     <hyperlink r:id="rId5" ref="B44"/>
-    <hyperlink r:id="rId6" ref="B60"/>
-    <hyperlink r:id="rId7" ref="B121"/>
+    <hyperlink r:id="rId6" ref="B55"/>
+    <hyperlink r:id="rId7" ref="B60"/>
+    <hyperlink r:id="rId8" ref="B121"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the thirteen days of el salvador
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -50,7 +50,7 @@
 &lt;p&gt;
 International scientific collaboration is essential to support global and regional efforts to protect marine biodiversity in areas within and beyond national jurisdiction. Several scientific programs and initiatives, such as the International Census of Marine Life Programme or the recently launched UN Decade of Ocean Science take the need to enhance scientific cooperation across regions into account to close data gaps, align research programs, and support conservation efforts. &lt;br&gt;
 Marine biodiversity research spans different spatial and temporal scales to assess global biodiversity loss patterns and is considered one of the most complex scientific fields to have emerged in recent decades [10]. As a big science, it ties together research teams, scientific infrastructures, laboratories, and equipment from different countries and regions of the world. While international scientific collaboration seems to be inherent to the marine biodiversity field, it is also highly encouraged by the United Nations Convention on the Law of the Sea (UNCLOS). &lt;br&gt;
-For more explanation of the methodological approach to researching marine biodiversity science bibliometrically, please refer to the  &lt;a href="https://www.sciencedirect.com/science/article/pii/S0308597X20309659"&gt;paper&lt;/a&gt; by Tolochko &amp; Vadrot (2021).
+For more explanation of the methodological approach to researching marine biodiversity science bibliometrically, please refer to the  &lt;a href="https://www.sciencedirect.com/science/article/pii/S0308597X20309659"&gt;paper by Tolochko &amp; Vadrot (2021)&lt;/a&gt; .
 &lt;p&gt;This section informs about the bibliometric analysis of marine biodiversity sciences.</t>
   </si>
   <si>
@@ -96,7 +96,7 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t>"&gt;paper&lt;/a&gt; by Tessnow-von Wysocki &amp; Vadrot (2021).
+      <t>"&gt;paper by Tessnow-von Wysocki &amp; Vadrot (2021)&lt;/a&gt; .
 &lt;p&gt;This section informs about the ongoing ethnographic work at the UN BBNJ negotiations.&lt;/p&gt;</t>
     </r>
   </si>
@@ -104,7 +104,42 @@
     <t>usa</t>
   </si>
   <si>
-    <t>The USA has an extensive network of ocean research facilities and labroratories. The National Association of Marine Labroratories counts with 104 member marine labroratories [1]. The various institutions in the USA are reported to posses marine research vessels, out of which NOAA posseses 19 and the US navy 10 vessels.</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>The USA has an extensive network of ocean research facilities and labroratories. The &lt;a href="https://www.naml.org/"&gt;National Association of Marine Labroratories counts with 104 member marine labroratories&lt;/a&gt;. The various institutions in the USA are reported to posses marine research vessels, out of which NOAA posseses 19 and the US navy 10 vessels.
+&lt;p&gt;
+Sources:
+[1] &lt;br&gt;&lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://www.naml.org/</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>"&lt;/a&gt;&lt;/br&gt;</t>
+    </r>
   </si>
   <si>
     <t>eu</t>
@@ -119,7 +154,8 @@
       <t>Managing and preventing the loss of biodiversity became a political topic in the EU in the 1990s. The European Environment Agency (EEA) observed extensive biodiversity loss across the European Community in a report putting pressure on governments to commonly act against these developments (EEA, Report for the Review of the Fifth Environmental Action Programme, 1995). On a global level, the Commission listed the biodiversity loss as one of the seven serious environmental problems facing the Union (CEC, Europe’s Environment: What Directions for the Future? The Global Assessment of the European Community Programme of Policy and Action in Relation to the Environment and Sustainable Development: ‘Towards Sustainability’,1999). Accordingly, the European Community was not only a major force in the negotiation of the CBD but also signed it already in 1992.
  In 2010, the EU identified halting the global loss of biodiversity by 2020 as one of its key priorities. A review in 2015 found that although the EU is the largest financial donor and has increased resources for global biodiversity, current progress is insufficient in reducing the impacts of EU consumption patterns on global biodiversity (EU, Biodiversity Strategy 2020 Midterm Review, 2015). The EU has been a supporter of multilateral approaches, openly addressing developing countries concerns about the fair and equitable sharing of benefits and as such it played an active role in the negotiation of the Nagoya Protocol. 
  In the EU there are about 230 research institutes out of which 55 are located in the UK, 46 in Germany and 29 in France &lt;p&gt;&lt;a href="http://www.marenet.de/MareNet/europe.html"&gt;[1]&lt;/a&gt;&lt;/p&gt; . There are currently 99 research vessels in Europe which are run 62 different research vessel operators in 23 countries [2]. Nevertheless, the distribution of vessels in Europe is not uniform. Three countries each operate 11 vessels (France, Germany and Norway), three countries operate between 7 and 9 vessels (UK, Spain and Portugal), and the remaining 17 countries operate five vessels or fewer [2]. 
-[1]  &lt;p&gt;&lt;a href="http://www.marenet.de/MareNet/europe.html"&gt;</t>
+[1]  &lt;br&gt;&lt;a href="http://www.marenet.de/MareNet/europe.html"&lt;/a&gt;&lt;/br&gt;  
+[2] &lt;br&gt;&lt;a href="</t>
     </r>
     <r>
       <rPr>
@@ -128,7 +164,7 @@
         <sz val="11.0"/>
         <u/>
       </rPr>
-      <t>http://www.marenet.de/MareNet/europe.html</t>
+      <t>https://www.marineboard.eu/sites/marineboard.eu/files/public/publication/EMB_PB7_Research_Vessels_Web_v4_0.pdf</t>
     </r>
     <r>
       <rPr>
@@ -136,8 +172,7 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve">&lt;/a&gt;&lt;/p&gt;  
-[2] https://www.marineboard.eu/sites/marineboard.eu/files/public/publication/EMB_PB7_Research_Vessels_Web_v4_0.pdf        </t>
+      <t xml:space="preserve">" &lt;/a&gt;&lt;/br&gt; </t>
     </r>
   </si>
   <si>
@@ -157,15 +192,86 @@
       </rPr>
       <t xml:space="preserve">Brazil is a country with strong interests in ocean issues. Its Exclusive Economic Zone encompasses 4.5 million km2 - called the Blue Amazon (Amazonia Azul) - which equals over 50% of the country’s land surface. 
  Its waters are governed by the Brazilian Interministerial Commission for Sea Resources (Comissão Interministerial para os Recursos do Mar - CIRM) which was established in 1974 and is coordinated and administred by the Navy. 
- The Brazilian government, through the Brazilian Interministerial Commission for Sea Resources (CIRM), has established the National Research Network in Marine Biotechnology (BiotecMar) which has 12 institutes in the area of biodiversity [1] and the Technical Group for Marine Science Education and Research (Grupo Técnico Formação de Recursos Humanos em Ciências do Mar – PPG-MAR) which aims to train "human resources capable of helping Brazil to develop scientific and technological research capacities, to promote the sustainable use of resources in national and international waters" [2]. The Brazilian Navy counts with 11 research vessels [3], the newest of which was unveiled in 2015. In the last years, further 4 research vessels (named Ciências do Mar I-IV) were handed directly to universities conducting relevant marine scientific research - Universidade Federal do Rio Grande (FURG) in 2017, Universidade Federal do Maranhão (UFMA) in 2018, Universidade Federal Fluminense (UFF) in 2019 [4] and Universidade Federal de Pernambuco in 2020 [5]. 
+ &lt;p&gt;
+The Brazilian government, through the Brazilian Interministerial Commission for Sea Resources (CIRM), has established the National Research Network in Marine Biotechnology (BiotecMar) which has 12 institutes in the area of biodiversity [1] and the Technical Group for Marine Science Education and Research (Grupo Técnico Formação de Recursos Humanos em Ciências do Mar – PPG-MAR) which aims to train "human resources capable of helping Brazil to develop scientific and technological research capacities, to promote the sustainable use of resources in national and international waters" [2]. The Brazilian Navy counts with 11 research vessels [3], the newest of which was unveiled in 2015. In the last years, further 4 research vessels (named Ciências do Mar I-IV) were handed directly to universities conducting relevant marine scientific research - Universidade Federal do Rio Grande (FURG) in 2017, Universidade Federal do Maranhão (UFMA) in 2018, Universidade Federal Fluminense (UFF) in 2019 [4] and Universidade Federal de Pernambuco in 2020 [5]. 
+ &lt;p&gt;
  14 universities in Brazil have oceanography departments or institutes that conduct marine scientific research, among which some universities possess specialized institutes or faculties: the Instituto Oceanográfico at the Universidade of Sao Paolo (Instituto Oceanográfico da Universidade de Sao Paulo (IOUSP), the Center for Marine Studies (“Centro de Estudos do Mar” – CEM) at the Federal University of Parana, the Faculty of Oceanography at the State University Rio de Janeiro (FAOC - Faculdade de Oceanografia da UERJ) and the Institute of Marine Sciences ("Instituto de Ciências do Mar" – LABOMAR) at the Federal University of Ceará). Brazilian universities offer 40 graduation courses and 28 post-graduation pogrammes related to marine sciences [6]. 
+ &lt;p&gt;
  Sources:
- [1] www.biotecmar.sage.coppe.ufrj.br 
- [2] https://cienciasdomarbrasil.furg.br/
- [3] https://www.marinha.mil.br/meios-navais
- [4] http://www.uff.br/?q=noticias/06-11-2018/navio-escola-da-uff-ampliara-desenvolvimento-tecnologico-nas-ciencias-do-mar
- [5] https://tapioca.ird.fr/embarcacao-ciencias-mar-iv-chega-neste-semestre-ao-porto-recife/
- [6] </t>
+ [1]&lt;br&gt;&lt;a href=" </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>www.biotecmar.sage.coppe.ufrj.br</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">" &lt;/a&gt;&lt;/br&gt; 
+ [2]&lt;br&gt;&lt;a href=" </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://cienciasdomarbrasil.furg.br</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>"&lt;/a&gt;&lt;/br&gt;
+ [3] &lt;br&gt;&lt;a href="</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://www.marinha.mil.br/meios-navais</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>"&lt;/a&gt;&lt;/br&gt;
+ [4] &lt;br&gt;&lt;a href="http://www.uff.br/?q=noticias/06-11-2018/navio-escola-da-uff-ampliara-desenvolvimento-tecnologico-nas-ciencias-do-mar"&lt;/a&gt;&lt;/br&gt;
+ [5] &lt;br&gt;&lt;a href="</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://tapioca.ird.fr/embarcacao-ciencias-mar-iv-chega-neste-semestre-ao-porto-recife</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>"&lt;/a&gt;&lt;/br&gt;
+ [6] &lt;br&gt;&lt;a href="</t>
     </r>
     <r>
       <rPr>
@@ -175,6 +281,14 @@
         <u/>
       </rPr>
       <t>https://www.marinha.mil.br/secirm/psrm/ppgmar</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>"&lt;/a&gt;&lt;/br&gt;</t>
     </r>
   </si>
   <si>
@@ -217,31 +331,35 @@
       <rPr>
         <color rgb="FF000000"/>
       </rPr>
-      <t>ce:</t>
+      <t>ces:</t>
     </r>
     <r>
       <rPr/>
-      <t xml:space="preserve"> 
-[1]http://medomed.org/wp-content/uploads/a2p.cache.algeria-biodiversity-conservation-data.pdf
+      <t xml:space="preserve">
+[1]&lt;br&gt;&lt;a href="http://medomed.org/wp-content/uploads/a2p.cache.algeria-biodiversity-conservation-data.pdf"&lt;/a&gt;&lt;/br&gt; 
 </t>
     </r>
     <r>
       <rPr>
         <color rgb="FF000000"/>
       </rPr>
-      <t xml:space="preserve">[2]https://medomed.org/countries/algeria/
+      <t xml:space="preserve">[2]&lt;br&gt;&lt;a href="https://medomed.org/countries/algeria/"&lt;/a&gt;&lt;/br&gt; 
 </t>
     </r>
     <r>
       <rPr/>
-      <t>[3]</t>
+      <t>[3]&lt;br&gt;&lt;a href="</t>
     </r>
     <r>
       <rPr>
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>http://www.vliz.be/events/marbena/Docs/final/MARBENAstatementsBiodiversityandSMEScontributionbySandSEMediterranean.pdf</t>
+      <t>http://www.vliz.be/events/marbena/Docs/final/MARBENAstatementsBiodiversityandSMEScontributionbySandSEMediterranean.pdf"</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">&lt;/a&gt;&lt;/br&gt; </t>
     </r>
   </si>
   <si>
@@ -373,21 +491,21 @@
       <rPr/>
       <t>Continental South Africa has a coastline of some 3,650 km and an Exclusive Economic Zone (EEZ) of just over 1 million km2. Waters in the EEZ extend to a depth of 5,700 m, with more than 65% deeper than 2,000 m. Despite its status as a developing nation, South Africa has a relatively strong history of marine taxonomic research and maintains comprehensive and well-curated museum collections totaling over 291,000 records. Over 3 million locality records from more than 23,000 species have been lodged in the regional AfrOBIS (African Ocean Biogeographic Information System) data center (which stores data from a wider African region). A large number of regional guides to the marine fauna and flora are also available and are listed. [1]
 South Africa has at least on active research vessel the S.A. Agulhas II.
-Sources: 
-[</t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF000000"/>
-      </rPr>
-      <t xml:space="preserve">1] </t>
+Sources: Continental South Africa has a coastline of some 3,650 km and an Exclusive Economic Zone (EEZ) of just over 1 million km2. Waters in the EEZ extend to a depth of 5,700 m, with more than 65% deeper than 2,000 m. Despite its status as a developing nation, South Africa has a relatively strong history of marine taxonomic research and maintains comprehensive and well-curated museum collections totaling over 291,000 records. Over 3 million locality records from more than 23,000 species have been lodged in the regional AfrOBIS (African Ocean Biogeographic Information System) data center (which stores data from a wider African region). A large number of regional guides to the marine fauna and flora are also available and are listed. [1]
+South Africa has at least on active research vessel the S.A. Agulhas II.
+Sources:  
+[1]  &lt;br&gt;&lt;a href="</t>
     </r>
     <r>
       <rPr>
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0012008</t>
+      <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0012008"</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">&lt;/a&gt;&lt;/br&gt; </t>
     </r>
   </si>
   <si>
@@ -1630,7 +1748,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6"/>
@@ -30427,14 +30545,15 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="B4"/>
-    <hyperlink r:id="rId3" ref="B5"/>
-    <hyperlink r:id="rId4" ref="B6"/>
-    <hyperlink r:id="rId5" ref="B44"/>
-    <hyperlink r:id="rId6" ref="B55"/>
-    <hyperlink r:id="rId7" ref="B60"/>
-    <hyperlink r:id="rId8" ref="B121"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="B5"/>
+    <hyperlink r:id="rId5" ref="B6"/>
+    <hyperlink r:id="rId6" ref="B44"/>
+    <hyperlink r:id="rId7" ref="B55"/>
+    <hyperlink r:id="rId8" ref="B60"/>
+    <hyperlink r:id="rId9" ref="B121"/>
   </hyperlinks>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>